<commit_message>
added EEBO/TCP counts to spreadsheet
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="13880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14900" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TESimplespreadsheet.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="130406" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="163">
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>merge with milestone</t>
+  </si>
+  <si>
+    <t>merge. Replace with empty ref</t>
+  </si>
+  <si>
+    <t>merge into q?</t>
+  </si>
+  <si>
+    <t>merge with hi</t>
+  </si>
+  <si>
+    <t>?? would need delSpan too</t>
+  </si>
+  <si>
+    <t>hard to distinguish from q sometimes</t>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
   <si>
     <t>element</t>
   </si>
@@ -481,34 +510,13 @@
   </si>
   <si>
     <t>caesura</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>merge with milestone</t>
-  </si>
-  <si>
-    <t>merge. Replace with empty ref</t>
-  </si>
-  <si>
-    <t>merge into q?</t>
-  </si>
-  <si>
-    <t>merge with hi</t>
-  </si>
-  <si>
-    <t>?? would need delSpan too</t>
-  </si>
-  <si>
-    <t>hard to distinguish from q sometimes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -553,6 +561,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -571,28 +588,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -917,231 +933,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18">
       <c r="A2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="18">
       <c r="A3" s="3" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="18">
       <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="4">
+        <v>521192</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="18">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="18">
       <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1809</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="18">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18">
       <c r="A8" s="3" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="18">
       <c r="A9" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="18">
       <c r="A10" s="3" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>159</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18">
       <c r="A11" s="3" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1149,1133 +1167,1133 @@
     </row>
     <row r="12" spans="1:7" ht="18">
       <c r="A12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>80</v>
+      </c>
+      <c r="B12" s="3">
+        <v>60149</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="18">
       <c r="A13" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>99</v>
+      </c>
+      <c r="B13" s="4">
+        <v>20843</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="18">
       <c r="A14" s="3" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="18">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="18">
       <c r="A16" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="B16" s="4">
+        <v>89899</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="18">
       <c r="A17" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>82</v>
+      </c>
+      <c r="B17" s="4">
+        <v>10046</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="18">
       <c r="A18" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="18">
       <c r="A19" s="3" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>155</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18">
       <c r="A20" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="18">
       <c r="A21" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="18">
       <c r="A22" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" ht="18">
       <c r="A23" s="3" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" ht="18">
       <c r="A24" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>8</v>
+        <v>105</v>
+      </c>
+      <c r="B24" s="4">
+        <v>3478371</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" ht="18">
       <c r="A25" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" ht="18">
       <c r="A26" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" ht="18">
       <c r="A27" s="3" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" ht="18">
       <c r="A28" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>8</v>
+        <v>83</v>
+      </c>
+      <c r="B28" s="4">
+        <v>102946</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="18">
       <c r="A29" s="3" t="s">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18">
       <c r="A30" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" ht="18">
       <c r="A31" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18">
       <c r="A32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="4">
+        <v>55863</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" ht="18">
       <c r="A33" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>84</v>
+      </c>
+      <c r="B33" s="4">
+        <v>45062</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" ht="18">
       <c r="A34" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" ht="18">
       <c r="A35" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" ht="18">
       <c r="A36" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>8</v>
+        <v>108</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1299500</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" ht="18">
       <c r="A37" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" ht="18">
       <c r="A38" s="3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" ht="18">
       <c r="A39" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" ht="18">
       <c r="A40" s="3" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" ht="18">
       <c r="A41" s="3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" ht="18">
       <c r="A42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>8</v>
+        <v>71</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" ht="18">
       <c r="A43" s="3" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18">
       <c r="A44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>8</v>
+        <v>72</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" ht="18">
       <c r="A45" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="B45" s="4">
+        <v>34583</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="18">
       <c r="A46" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="18">
       <c r="A47" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>8</v>
+        <v>75</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" ht="18">
       <c r="A48" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>8</v>
+        <v>109</v>
+      </c>
+      <c r="B48" s="4">
+        <v>19247</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" ht="18">
       <c r="A49" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" ht="18">
       <c r="A50" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>8</v>
+        <v>78</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" ht="18">
       <c r="A51" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>6</v>
+        <v>111</v>
+      </c>
+      <c r="B51" s="6">
+        <v>34511</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="18">
       <c r="A52" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="18">
       <c r="A53" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18">
       <c r="A54" s="3" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" ht="18">
       <c r="A55" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>8</v>
+        <v>114</v>
+      </c>
+      <c r="B55" s="4">
+        <v>40756</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" ht="18">
       <c r="A56" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" ht="18">
       <c r="A57" s="3" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" ht="18">
       <c r="A58" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="B58" s="4">
+        <v>108894</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" ht="18">
       <c r="A59" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18">
       <c r="A60" s="3" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18">
       <c r="A61" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" ht="18">
       <c r="A62" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>8</v>
+        <v>124</v>
+      </c>
+      <c r="B62" s="4">
+        <v>2311</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" ht="18">
       <c r="A63" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>8</v>
+        <v>125</v>
+      </c>
+      <c r="B63" s="4">
+        <v>1541470</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" ht="18">
       <c r="A64" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>8</v>
+        <v>126</v>
+      </c>
+      <c r="B64" s="4">
+        <v>46780581</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="18">
       <c r="A65" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>8</v>
+        <v>92</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="18">
       <c r="A66" s="3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G66" s="3"/>
     </row>
     <row r="67" spans="1:7" ht="18">
       <c r="A67" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" ht="18">
       <c r="A68" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>8</v>
+        <v>94</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="18">
       <c r="A69" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>8</v>
+        <v>128</v>
+      </c>
+      <c r="B69" s="4">
+        <v>10272751</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -2283,16 +2301,16 @@
     </row>
     <row r="70" spans="1:7" ht="18">
       <c r="A70" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>8</v>
+        <v>129</v>
+      </c>
+      <c r="B70" s="4">
+        <v>185529</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -2300,16 +2318,16 @@
     </row>
     <row r="71" spans="1:7" ht="18">
       <c r="A71" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>8</v>
+        <v>131</v>
+      </c>
+      <c r="B71" s="4">
+        <v>22738</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -2317,16 +2335,16 @@
     </row>
     <row r="72" spans="1:7" ht="18">
       <c r="A72" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>8</v>
+        <v>132</v>
+      </c>
+      <c r="B72" s="4">
+        <v>714182</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -2334,33 +2352,33 @@
     </row>
     <row r="73" spans="1:7" ht="18">
       <c r="A73" s="3" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="18">
       <c r="A74" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>8</v>
+        <v>133</v>
+      </c>
+      <c r="B74" s="4">
+        <v>319957</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -2368,264 +2386,264 @@
     </row>
     <row r="75" spans="1:7" ht="18">
       <c r="A75" s="3" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="18">
       <c r="A76" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="1:7" ht="18">
       <c r="A77" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18">
       <c r="A78" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>8</v>
+        <v>135</v>
+      </c>
+      <c r="B78" s="4">
+        <v>732115</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
     </row>
     <row r="79" spans="1:7" ht="18">
       <c r="A79" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G79" s="3"/>
     </row>
     <row r="80" spans="1:7" ht="18">
       <c r="A80" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G80" s="3"/>
     </row>
     <row r="81" spans="1:7" ht="18">
       <c r="A81" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
     </row>
     <row r="82" spans="1:7" ht="18">
       <c r="A82" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18">
       <c r="A83" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>8</v>
+        <v>136</v>
+      </c>
+      <c r="B83" s="4">
+        <v>4091422</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7" ht="18">
       <c r="A84" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
+      </c>
+      <c r="B84" s="4">
+        <v>66501</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G84" s="3"/>
     </row>
     <row r="85" spans="1:7" ht="18">
       <c r="A85" s="3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18">
       <c r="A86" s="3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G86" s="3"/>
     </row>
     <row r="87" spans="1:7" ht="18">
       <c r="A87" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>8</v>
+        <v>137</v>
+      </c>
+      <c r="B87" s="4">
+        <v>9793935</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
@@ -2633,16 +2651,16 @@
     </row>
     <row r="88" spans="1:7" ht="18">
       <c r="A88" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>8</v>
+        <v>139</v>
+      </c>
+      <c r="B88" s="4">
+        <v>4482600</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
@@ -2650,220 +2668,220 @@
     </row>
     <row r="89" spans="1:7" ht="18">
       <c r="A89" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G89" s="3"/>
     </row>
     <row r="90" spans="1:7" ht="18">
       <c r="A90" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18">
       <c r="A91" s="3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G91" s="3"/>
     </row>
     <row r="92" spans="1:7" ht="18">
       <c r="A92" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B92" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="G92" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18">
       <c r="A93" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>8</v>
+        <v>87</v>
+      </c>
+      <c r="B93" s="4">
+        <v>5048</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" ht="18">
       <c r="A94" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>8</v>
+        <v>115</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" ht="18">
       <c r="A95" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>8</v>
+        <v>43</v>
+      </c>
+      <c r="B95" s="3">
+        <v>634</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>156</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18">
       <c r="A96" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>8</v>
+        <v>117</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G96" s="3"/>
     </row>
     <row r="97" spans="1:7" ht="18">
       <c r="A97" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G97" s="3"/>
     </row>
     <row r="98" spans="1:7" ht="18">
       <c r="A98" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G98" s="3"/>
     </row>
     <row r="99" spans="1:7" ht="18">
       <c r="A99" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>8</v>
+        <v>142</v>
+      </c>
+      <c r="B99" s="3">
+        <v>108</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -2871,35 +2889,35 @@
     </row>
     <row r="100" spans="1:7" ht="18">
       <c r="A100" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>6</v>
+        <v>143</v>
+      </c>
+      <c r="B100" s="4">
+        <v>579010</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3" t="s">
-        <v>160</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="18">
       <c r="A101" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>8</v>
+        <v>144</v>
+      </c>
+      <c r="B101" s="4">
+        <v>3488</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
@@ -2907,637 +2925,637 @@
     </row>
     <row r="102" spans="1:7" ht="18">
       <c r="A102" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="G102" s="3"/>
     </row>
     <row r="103" spans="1:7" ht="18">
       <c r="A103" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G103" s="3"/>
     </row>
     <row r="104" spans="1:7" ht="18">
       <c r="A104" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G104" s="3"/>
     </row>
     <row r="105" spans="1:7" ht="18">
       <c r="A105" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G105" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="18">
       <c r="A106" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>8</v>
+        <v>145</v>
+      </c>
+      <c r="B106" s="4">
+        <v>955765</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
     </row>
     <row r="107" spans="1:7" ht="18">
       <c r="A107" s="3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G107" s="3"/>
     </row>
     <row r="108" spans="1:7" ht="18">
       <c r="A108" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>8</v>
+        <v>88</v>
+      </c>
+      <c r="B108" s="4">
+        <v>54216</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G108" s="3"/>
     </row>
     <row r="109" spans="1:7" ht="18">
       <c r="A109" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>6</v>
+        <v>146</v>
+      </c>
+      <c r="B109" s="4">
+        <v>506546</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
     </row>
     <row r="110" spans="1:7" ht="18">
       <c r="A110" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G110" s="3"/>
     </row>
     <row r="111" spans="1:7" ht="18">
       <c r="A111" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>8</v>
+        <v>89</v>
+      </c>
+      <c r="B111" s="4">
+        <v>90170</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G111" s="3"/>
     </row>
     <row r="112" spans="1:7" ht="18">
       <c r="A112" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>6</v>
+        <v>44</v>
+      </c>
+      <c r="B112" s="3">
+        <v>0</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>157</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="18">
       <c r="A113" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>8</v>
+        <v>130</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G113" s="3"/>
     </row>
     <row r="114" spans="1:7" ht="18">
       <c r="A114" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="B114" s="4">
+        <v>1479103</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
     </row>
     <row r="115" spans="1:7" ht="18">
       <c r="A115" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G115" s="3"/>
     </row>
     <row r="116" spans="1:7" ht="18">
       <c r="A116" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>8</v>
+        <v>148</v>
+      </c>
+      <c r="B116" s="4">
+        <v>1471913</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
     </row>
     <row r="117" spans="1:7" ht="18">
       <c r="A117" s="3" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
     </row>
     <row r="118" spans="1:7" ht="18">
       <c r="A118" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>8</v>
+        <v>150</v>
+      </c>
+      <c r="B118" s="4">
+        <v>220000</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
     </row>
     <row r="119" spans="1:7" ht="18">
       <c r="A119" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G119" s="3"/>
     </row>
     <row r="120" spans="1:7" ht="18">
       <c r="A120" s="3" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="18">
       <c r="A121" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>8</v>
+        <v>151</v>
+      </c>
+      <c r="B121" s="4">
+        <v>58531</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
     </row>
     <row r="122" spans="1:7" ht="18">
       <c r="A122" s="3" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
     </row>
     <row r="123" spans="1:7" ht="18">
       <c r="A123" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>8</v>
+        <v>138</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="G123" s="3"/>
     </row>
     <row r="124" spans="1:7" ht="18">
       <c r="A124" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="G124" s="3"/>
     </row>
     <row r="125" spans="1:7" ht="18">
       <c r="A125" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>8</v>
+        <v>154</v>
+      </c>
+      <c r="B125" s="4">
+        <v>57697</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
     </row>
     <row r="126" spans="1:7" ht="18">
       <c r="A126" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>8</v>
+        <v>140</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G126" s="3"/>
     </row>
     <row r="127" spans="1:7" ht="18">
       <c r="A127" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>8</v>
+        <v>155</v>
+      </c>
+      <c r="B127" s="3">
+        <v>0</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
     </row>
     <row r="128" spans="1:7" ht="15" customHeight="1">
       <c r="A128" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F128" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F128" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="G128" s="3"/>
     </row>
     <row r="129" spans="1:7" s="3" customFormat="1" ht="18">
       <c r="A129" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="130" spans="1:7" s="3" customFormat="1" ht="18">
       <c r="A130" s="3" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="131" spans="1:7" s="3" customFormat="1" ht="18">
       <c r="A131" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B131" s="4">
+        <v>58254</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F131" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E131" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="132" spans="1:7" s="3" customFormat="1" ht="18">
       <c r="A132" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="B132" s="4">
+        <v>4022</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="133" spans="1:7" s="3" customFormat="1" ht="18">
       <c r="A133" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>6</v>
+        <v>52</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="3" customFormat="1" ht="18">
@@ -3553,10 +3571,10 @@
   <sortState ref="A3:G134">
     <sortCondition ref="A3:A134"/>
   </sortState>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
updated from spreadsheet; stop validate failing on error
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="0" windowWidth="20320" windowHeight="17400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37180" windowHeight="19280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TESimplespreadsheet.csv" sheetId="1" r:id="rId1"/>
@@ -515,9 +515,6 @@
     <t>Tite</t>
   </si>
   <si>
-    <t>handshift</t>
-  </si>
-  <si>
     <t>num</t>
   </si>
   <si>
@@ -537,6 +534,9 @@
   </si>
   <si>
     <t>do we need this</t>
+  </si>
+  <si>
+    <t>handShift</t>
   </si>
 </sst>
 </file>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136:XFD136"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -986,7 +986,7 @@
         <v>163</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>11</v>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18">
@@ -2359,7 +2359,7 @@
     </row>
     <row r="63" spans="1:9" ht="18">
       <c r="A63" s="3" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4" t="s">
@@ -2827,7 +2827,7 @@
     </row>
     <row r="85" spans="1:9" ht="18">
       <c r="A85" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="4" t="s">
@@ -2839,7 +2839,7 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="18">
@@ -3377,7 +3377,7 @@
     </row>
     <row r="109" spans="1:9" ht="18">
       <c r="A109" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
@@ -3830,7 +3830,7 @@
     </row>
     <row r="130" spans="1:9" ht="18">
       <c r="A130" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B130" s="5"/>
       <c r="C130" s="5" t="s">
@@ -3842,7 +3842,7 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="18">

</xml_diff>

<commit_message>
deal with teiHeader a bit differently, leave wrapper TEI in place
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37180" windowHeight="19280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37120" windowHeight="19220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TESimplespreadsheet.csv" sheetId="1" r:id="rId1"/>
@@ -527,9 +527,6 @@
     <t>rs</t>
   </si>
   <si>
-    <t>what about time</t>
-  </si>
-  <si>
     <t>do we need this?</t>
   </si>
   <si>
@@ -537,6 +534,9 @@
   </si>
   <si>
     <t>handShift</t>
+  </si>
+  <si>
+    <t>would need time too?</t>
   </si>
 </sst>
 </file>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18">
@@ -2359,7 +2359,7 @@
     </row>
     <row r="63" spans="1:9" ht="18">
       <c r="A63" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4" t="s">
@@ -2839,7 +2839,7 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="18">
@@ -3178,7 +3178,7 @@
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>15</v>
@@ -3842,7 +3842,7 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="18">

</xml_diff>

<commit_message>
small changes to spreadsheet, agenda for committee
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37120" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="14000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TESimplespreadsheet.csv" sheetId="1" r:id="rId1"/>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E2" sqref="A2:I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1006,36 +1006,36 @@
     </row>
     <row r="2" spans="1:9" ht="18">
       <c r="A2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0</v>
+        <v>93</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="18">
       <c r="A3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B3" s="4">
+        <v>521192</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1043,83 +1043,87 @@
         <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="18">
       <c r="A4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="4">
-        <v>521192</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="18">
       <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1809</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="18">
       <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1809</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="18">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>15</v>
@@ -1135,16 +1139,12 @@
       <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="18">
       <c r="A8" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
@@ -1165,34 +1165,32 @@
     </row>
     <row r="9" spans="1:9" ht="18">
       <c r="A9" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="18">
       <c r="A10" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1201,15 +1199,15 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="18">
       <c r="A11" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="B11" s="3">
+        <v>60149</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
@@ -1218,21 +1216,25 @@
       <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="18">
       <c r="A12" s="3" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B12" s="3">
-        <v>60149</v>
+        <v>0</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>17</v>
@@ -1240,9 +1242,7 @@
       <c r="G12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="18">
@@ -4003,8 +4003,8 @@
       <c r="I138"/>
     </row>
   </sheetData>
-  <sortState ref="A3:G134">
-    <sortCondition ref="A3:A134"/>
+  <sortState ref="A2:I137">
+    <sortCondition ref="A2:A137"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
numbers 4 ota and dta in stylesheet
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37120" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TESimplespreadsheet.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="176">
   <si>
     <t>code</t>
   </si>
@@ -537,6 +537,18 @@
   </si>
   <si>
     <t>would need time too?</t>
+  </si>
+  <si>
+    <t>OTAnrs</t>
+  </si>
+  <si>
+    <t>surface</t>
+  </si>
+  <si>
+    <t>facsimile</t>
+  </si>
+  <si>
+    <t>DTAnrs</t>
   </si>
 </sst>
 </file>
@@ -630,12 +642,17 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -961,21 +978,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.83203125" customWidth="1"/>
-    <col min="9" max="9" width="45" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.875" customWidth="1"/>
+    <col min="11" max="11" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="18">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -992,19 +1009,25 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18">
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>97</v>
       </c>
@@ -1016,16 +1039,19 @@
       <c r="E2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="18">
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>93</v>
       </c>
@@ -1039,16 +1065,19 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
+      <c r="F3">
+        <v>60496</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="18">
+        <v>17</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1060,18 +1089,24 @@
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
+      <c r="F4">
+        <v>7015</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4">
+        <v>69</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="18">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1083,18 +1118,24 @@
       <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
+      <c r="F5" s="3">
+        <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="18">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1106,18 +1147,21 @@
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
+      <c r="F6">
+        <v>137</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="18">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>54</v>
       </c>
@@ -1129,20 +1173,21 @@
       <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18">
+    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>95</v>
       </c>
@@ -1154,16 +1199,17 @@
       <c r="E8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="18">
+        <v>15</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>96</v>
       </c>
@@ -1175,16 +1221,17 @@
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="18">
+        <v>15</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>160</v>
       </c>
@@ -1196,16 +1243,17 @@
       <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18">
+    <row r="11" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>161</v>
       </c>
@@ -1215,14 +1263,17 @@
       <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="F11">
+        <v>29</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="18">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>80</v>
       </c>
@@ -1234,18 +1285,24 @@
       <c r="E12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>17</v>
+      <c r="F12">
+        <v>1795</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12">
+        <v>3001</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="18">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>99</v>
       </c>
@@ -1257,16 +1314,22 @@
       <c r="E13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>17</v>
+      <c r="F13">
+        <v>7734</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="18">
+      <c r="H13">
+        <v>753</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>101</v>
       </c>
@@ -1278,16 +1341,22 @@
       <c r="E14" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>17</v>
+      <c r="F14">
+        <v>16180</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="18">
+      <c r="H14">
+        <v>4470</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -1300,15 +1369,16 @@
         <v>40</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="G15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" ht="18">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>102</v>
       </c>
@@ -1320,16 +1390,22 @@
       <c r="E16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>17</v>
+      <c r="F16">
+        <v>9246</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" ht="18">
+      <c r="H16">
+        <v>1378</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>82</v>
       </c>
@@ -1341,18 +1417,24 @@
       <c r="E17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>17</v>
+      <c r="F17">
+        <v>3549</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17">
+        <v>1228</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" ht="18">
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -1367,15 +1449,16 @@
         <v>16</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="G18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" ht="18">
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>162</v>
       </c>
@@ -1387,16 +1470,19 @@
       <c r="E19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3" t="s">
+      <c r="F19">
+        <v>30299</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="18">
+    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1410,18 +1496,22 @@
       <c r="E20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20">
+        <v>58</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" ht="18">
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1435,18 +1525,24 @@
       <c r="E21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>17</v>
+      <c r="F21">
+        <v>90</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21">
+        <v>903</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="18">
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1460,18 +1556,24 @@
       <c r="E22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>17</v>
+      <c r="F22">
+        <v>4</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22">
+        <v>87</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" ht="18">
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>104</v>
       </c>
@@ -1485,16 +1587,20 @@
       <c r="E23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" ht="18">
+        <v>15</v>
+      </c>
+      <c r="H23">
+        <v>27874</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>105</v>
       </c>
@@ -1506,16 +1612,22 @@
       <c r="E24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>17</v>
+      <c r="F24">
+        <v>138105</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" ht="18">
+      <c r="H24">
+        <v>37698</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>60</v>
       </c>
@@ -1528,15 +1640,16 @@
         <v>40</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="3" t="s">
+      <c r="G25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="18">
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
@@ -1548,18 +1661,24 @@
       <c r="E26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>17</v>
+      <c r="F26">
+        <v>770</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26">
+        <v>10128</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" ht="18">
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>106</v>
       </c>
@@ -1571,16 +1690,22 @@
       <c r="E27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>15</v>
+      <c r="F27">
+        <v>155</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" ht="18">
+        <v>15</v>
+      </c>
+      <c r="H27">
+        <v>5566</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>83</v>
       </c>
@@ -1592,18 +1717,24 @@
       <c r="E28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>17</v>
+      <c r="F28">
+        <v>9414</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28">
+        <v>1806</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" ht="18">
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -1613,16 +1744,19 @@
       <c r="E29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3" t="s">
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="18">
+    <row r="30" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -1634,18 +1768,24 @@
       <c r="E30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>17</v>
+      <c r="F30">
+        <v>505</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30">
+        <v>7292</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" ht="18">
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>57</v>
       </c>
@@ -1659,20 +1799,21 @@
       <c r="E31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="K31" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="18">
+    <row r="32" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>107</v>
       </c>
@@ -1684,18 +1825,24 @@
       <c r="E32" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>17</v>
+      <c r="F32">
+        <v>7734</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="3"/>
+      <c r="H32">
+        <v>117</v>
+      </c>
       <c r="I32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="18">
+    <row r="33" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>84</v>
       </c>
@@ -1707,18 +1854,24 @@
       <c r="E33" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>17</v>
+      <c r="F33">
+        <v>7247</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33">
+        <v>3641</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" ht="18">
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>29</v>
       </c>
@@ -1730,18 +1883,21 @@
       <c r="E34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>17</v>
+      <c r="F34">
+        <v>15</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" ht="18">
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
@@ -1753,16 +1909,19 @@
       <c r="E35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3" t="s">
+      <c r="F35">
+        <v>125150</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" ht="18">
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>108</v>
       </c>
@@ -1774,16 +1933,22 @@
       <c r="E36" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>17</v>
+      <c r="F36">
+        <v>85352</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" ht="18">
+      <c r="H36">
+        <v>124593</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>67</v>
       </c>
@@ -1795,18 +1960,24 @@
       <c r="E37" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>17</v>
+      <c r="F37">
+        <v>381</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37">
+        <v>1021</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" ht="18">
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>69</v>
       </c>
@@ -1818,18 +1989,24 @@
       <c r="E38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>17</v>
+      <c r="F38">
+        <v>6</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38">
+        <v>1105</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" ht="18">
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>70</v>
       </c>
@@ -1841,18 +2018,22 @@
       <c r="E39" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39">
+        <v>15</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" ht="18">
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>73</v>
       </c>
@@ -1864,18 +2045,24 @@
       <c r="E40" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>17</v>
+      <c r="F40">
+        <v>223</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40">
+        <v>1159</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:9" ht="18">
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>74</v>
       </c>
@@ -1887,18 +2074,24 @@
       <c r="E41" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>17</v>
+      <c r="F41">
+        <v>349</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41">
+        <v>1427</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" ht="18">
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>71</v>
       </c>
@@ -1912,12 +2105,13 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3" t="s">
+      <c r="I42" s="3"/>
+      <c r="J42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" ht="18">
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>159</v>
       </c>
@@ -1927,16 +2121,19 @@
       <c r="E43" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3" t="s">
+      <c r="F43">
+        <v>6711</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="18">
+    <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>72</v>
       </c>
@@ -1950,12 +2147,13 @@
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3" t="s">
+      <c r="I44" s="3"/>
+      <c r="J44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" ht="18">
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>85</v>
       </c>
@@ -1967,18 +2165,24 @@
       <c r="E45" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>17</v>
+      <c r="F45">
+        <v>2645</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45">
+        <v>155</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" ht="18">
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>31</v>
       </c>
@@ -1990,18 +2194,22 @@
       <c r="E46" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46">
+        <v>69</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" ht="18">
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>75</v>
       </c>
@@ -2015,12 +2223,13 @@
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="3" t="s">
+      <c r="I47" s="3"/>
+      <c r="J47" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9" ht="18">
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>109</v>
       </c>
@@ -2032,16 +2241,19 @@
       <c r="E48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>17</v>
+      <c r="F48">
+        <v>1147</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:9" ht="18">
+        <v>17</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>110</v>
       </c>
@@ -2053,16 +2265,22 @@
       <c r="E49" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>17</v>
+      <c r="F49">
+        <v>5247</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" ht="18">
+      <c r="H49">
+        <v>23175</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>78</v>
       </c>
@@ -2076,12 +2294,13 @@
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="3" t="s">
+      <c r="I50" s="3"/>
+      <c r="J50" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="1:9" ht="18">
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>111</v>
       </c>
@@ -2095,16 +2314,22 @@
       <c r="E51" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>17</v>
+      <c r="F51">
+        <v>6120</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" ht="18">
+      <c r="H51">
+        <v>342</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>112</v>
       </c>
@@ -2116,16 +2341,22 @@
       <c r="E52" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>15</v>
+      <c r="F52">
+        <v>2365</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:9" ht="18">
+        <v>15</v>
+      </c>
+      <c r="H52">
+        <v>4462</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
@@ -2139,20 +2370,21 @@
       <c r="E53" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="K53" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="18">
+    <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>113</v>
       </c>
@@ -2164,16 +2396,20 @@
       <c r="E54" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:9" ht="18">
+        <v>15</v>
+      </c>
+      <c r="H54">
+        <v>27014</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+    </row>
+    <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>114</v>
       </c>
@@ -2185,16 +2421,22 @@
       <c r="E55" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>17</v>
+      <c r="F55">
+        <v>2815</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-    </row>
-    <row r="56" spans="1:9" ht="18">
+      <c r="H55">
+        <v>1040</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>116</v>
       </c>
@@ -2208,16 +2450,22 @@
       <c r="E56" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>17</v>
+      <c r="F56">
+        <v>15</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="1:9" ht="18">
+      <c r="H56">
+        <v>402921</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>120</v>
       </c>
@@ -2231,16 +2479,22 @@
       <c r="E57" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>17</v>
+      <c r="F57">
+        <v>489</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-    </row>
-    <row r="58" spans="1:9" ht="18">
+        <v>17</v>
+      </c>
+      <c r="H57">
+        <v>493</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>32</v>
       </c>
@@ -2252,18 +2506,24 @@
       <c r="E58" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>17</v>
+      <c r="F58">
+        <v>125202</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H58">
+        <v>6363</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I58" s="3"/>
-    </row>
-    <row r="59" spans="1:9" ht="18">
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>59</v>
       </c>
@@ -2277,20 +2537,21 @@
       <c r="E59" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F59" s="3"/>
       <c r="G59" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I59" s="3" t="s">
+      <c r="K59" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="18">
+    <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>121</v>
       </c>
@@ -2304,18 +2565,21 @@
       <c r="E60" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>17</v>
+      <c r="F60">
+        <v>45</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H60" s="3"/>
+        <v>17</v>
+      </c>
       <c r="I60" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="18">
+    <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>123</v>
       </c>
@@ -2327,16 +2591,19 @@
       <c r="E61" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>17</v>
+      <c r="F61">
+        <v>200</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-    </row>
-    <row r="62" spans="1:9" ht="18">
+        <v>17</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>124</v>
       </c>
@@ -2348,16 +2615,19 @@
       <c r="E62" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>17</v>
+      <c r="F62">
+        <v>71</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-    </row>
-    <row r="63" spans="1:9" ht="18">
+      <c r="I62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>170</v>
       </c>
@@ -2369,14 +2639,17 @@
         <v>15</v>
       </c>
       <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
+      <c r="F63" s="3">
+        <v>0</v>
+      </c>
       <c r="G63" s="3"/>
-      <c r="H63" s="3" t="s">
+      <c r="I63" s="3"/>
+      <c r="J63" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I63" s="3"/>
-    </row>
-    <row r="64" spans="1:9" ht="18">
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>125</v>
       </c>
@@ -2388,16 +2661,22 @@
       <c r="E64" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>17</v>
+      <c r="F64">
+        <v>115775</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-    </row>
-    <row r="65" spans="1:9" ht="18">
+      <c r="H64">
+        <v>144164</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>126</v>
       </c>
@@ -2409,16 +2688,22 @@
       <c r="E65" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>17</v>
+      <c r="F65">
+        <v>1419289</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-    </row>
-    <row r="66" spans="1:9" ht="18">
+      <c r="H65">
+        <v>2758132</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>92</v>
       </c>
@@ -2430,14 +2715,17 @@
       <c r="E66" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F66" s="3"/>
+      <c r="F66" s="3">
+        <v>0</v>
+      </c>
       <c r="G66" s="3"/>
-      <c r="H66" s="3" t="s">
+      <c r="I66" s="3"/>
+      <c r="J66" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I66" s="3"/>
-    </row>
-    <row r="67" spans="1:9" ht="18">
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>76</v>
       </c>
@@ -2449,18 +2737,24 @@
       <c r="E67" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>17</v>
+      <c r="F67">
+        <v>23</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="H67">
+        <v>72</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I67" s="3"/>
-    </row>
-    <row r="68" spans="1:9" ht="18">
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>127</v>
       </c>
@@ -2472,16 +2766,22 @@
       <c r="E68" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>17</v>
+      <c r="F68">
+        <v>188278</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="1:9" ht="18">
+      <c r="H68">
+        <v>229168</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>94</v>
       </c>
@@ -2493,14 +2793,17 @@
       <c r="E69" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F69" s="3"/>
+      <c r="F69" s="3">
+        <v>0</v>
+      </c>
       <c r="G69" s="3"/>
-      <c r="H69" s="3" t="s">
+      <c r="I69" s="3"/>
+      <c r="J69" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I69" s="3"/>
-    </row>
-    <row r="70" spans="1:9" ht="18">
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>128</v>
       </c>
@@ -2512,14 +2815,20 @@
       <c r="E70" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
+      <c r="F70">
+        <v>1428379</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70">
+        <v>631256</v>
+      </c>
       <c r="I70" s="3"/>
-    </row>
-    <row r="71" spans="1:9" ht="18">
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>129</v>
       </c>
@@ -2531,14 +2840,17 @@
       <c r="E71" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
+      <c r="F71">
+        <v>19570</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="1:9" ht="18">
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+    </row>
+    <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>131</v>
       </c>
@@ -2550,14 +2862,20 @@
       <c r="E72" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
+      <c r="F72">
+        <v>1508235</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H72">
+        <v>11923956</v>
+      </c>
       <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="1:9" ht="18">
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+    </row>
+    <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>132</v>
       </c>
@@ -2569,14 +2887,20 @@
       <c r="E73" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
+      <c r="F73">
+        <v>86396</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73">
+        <v>96717</v>
+      </c>
       <c r="I73" s="3"/>
-    </row>
-    <row r="74" spans="1:9" ht="18">
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+    </row>
+    <row r="74" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>100</v>
       </c>
@@ -2590,12 +2914,13 @@
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
-      <c r="H74" s="3" t="s">
+      <c r="I74" s="3"/>
+      <c r="J74" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I74" s="3"/>
-    </row>
-    <row r="75" spans="1:9" ht="18">
+      <c r="K74" s="3"/>
+    </row>
+    <row r="75" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>133</v>
       </c>
@@ -2607,14 +2932,20 @@
       <c r="E75" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F75" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
+      <c r="F75">
+        <v>17848</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75">
+        <v>28676</v>
+      </c>
       <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="1:9" ht="18">
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>134</v>
       </c>
@@ -2626,16 +2957,20 @@
       <c r="E76" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F76" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F76" s="3"/>
       <c r="G76" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-    </row>
-    <row r="77" spans="1:9" ht="18">
+        <v>15</v>
+      </c>
+      <c r="H76">
+        <v>26</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+    </row>
+    <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>103</v>
       </c>
@@ -2650,15 +2985,16 @@
         <v>40</v>
       </c>
       <c r="F77" s="3"/>
-      <c r="G77" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H77" s="3" t="s">
+      <c r="G77" s="3"/>
+      <c r="I77" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I77" s="3"/>
-    </row>
-    <row r="78" spans="1:9" ht="18">
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>45</v>
       </c>
@@ -2672,20 +3008,21 @@
       <c r="E78" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F78" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F78" s="3"/>
       <c r="G78" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H78" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J78" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I78" s="3" t="s">
+      <c r="K78" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="18">
+    <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>135</v>
       </c>
@@ -2697,16 +3034,22 @@
       <c r="E79" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F79" s="3" t="s">
-        <v>17</v>
+      <c r="F79">
+        <v>14639</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-    </row>
-    <row r="80" spans="1:9" ht="18">
+      <c r="H79">
+        <v>57816</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>39</v>
       </c>
@@ -2720,18 +3063,19 @@
       <c r="E80" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F80" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F80" s="3"/>
       <c r="G80" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H80" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J80" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I80" s="3"/>
-    </row>
-    <row r="81" spans="1:9" ht="18">
+      <c r="K80" s="3"/>
+    </row>
+    <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>41</v>
       </c>
@@ -2745,18 +3089,19 @@
       <c r="E81" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F81" s="3"/>
       <c r="G81" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H81" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J81" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I81" s="3"/>
-    </row>
-    <row r="82" spans="1:9" ht="18">
+      <c r="K81" s="3"/>
+    </row>
+    <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>55</v>
       </c>
@@ -2768,16 +3113,22 @@
       <c r="E82" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>17</v>
+      <c r="F82">
+        <v>2541</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="1:9" ht="18">
+      <c r="H82">
+        <v>3</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+    </row>
+    <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>61</v>
       </c>
@@ -2791,20 +3142,21 @@
       <c r="E83" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F83" s="3"/>
       <c r="G83" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H83" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J83" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I83" s="3" t="s">
+      <c r="K83" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="18">
+    <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>136</v>
       </c>
@@ -2816,16 +3168,22 @@
       <c r="E84" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>17</v>
+      <c r="F84">
+        <v>113910</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-    </row>
-    <row r="85" spans="1:9" ht="18">
+      <c r="H84">
+        <v>214219</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+    </row>
+    <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>164</v>
       </c>
@@ -2837,12 +3195,13 @@
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="3" t="s">
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="18">
+    <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>86</v>
       </c>
@@ -2854,18 +3213,24 @@
       <c r="E86" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F86" s="3" t="s">
-        <v>17</v>
+      <c r="F86">
+        <v>9727</v>
       </c>
       <c r="G86" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H86" s="3" t="s">
+      <c r="H86">
+        <v>531</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J86" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="1:9" ht="18">
+      <c r="K86" s="3"/>
+    </row>
+    <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>62</v>
       </c>
@@ -2879,20 +3244,21 @@
       <c r="E87" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F87" s="3"/>
       <c r="G87" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H87" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I87" s="3" t="s">
+      <c r="K87" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="18">
+    <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>33</v>
       </c>
@@ -2904,18 +3270,24 @@
       <c r="E88" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>17</v>
+      <c r="F88">
+        <v>274</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H88" s="3" t="s">
+      <c r="H88">
+        <v>2772</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J88" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I88" s="3"/>
-    </row>
-    <row r="89" spans="1:9" ht="18">
+      <c r="K88" s="3"/>
+    </row>
+    <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>137</v>
       </c>
@@ -2927,14 +3299,20 @@
       <c r="E89" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F89" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
+      <c r="F89">
+        <v>1099529</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H89">
+        <v>736405</v>
+      </c>
       <c r="I89" s="3"/>
-    </row>
-    <row r="90" spans="1:9" ht="18">
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+    </row>
+    <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>139</v>
       </c>
@@ -2946,14 +3324,20 @@
       <c r="E90" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F90" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
+      <c r="F90">
+        <v>362846</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H90">
+        <v>383056</v>
+      </c>
       <c r="I90" s="3"/>
-    </row>
-    <row r="91" spans="1:9" ht="18">
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+    </row>
+    <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>50</v>
       </c>
@@ -2967,18 +3351,19 @@
       <c r="E91" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F91" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F91" s="3"/>
       <c r="G91" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H91" s="3" t="s">
+      <c r="I91" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J91" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I91" s="3"/>
-    </row>
-    <row r="92" spans="1:9" ht="18">
+      <c r="K91" s="3"/>
+    </row>
+    <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>63</v>
       </c>
@@ -2994,20 +3379,24 @@
       <c r="E92" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F92" s="3"/>
       <c r="G92" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H92">
+        <v>27489</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J92" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I92" s="3" t="s">
+      <c r="K92" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="18">
+    <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>42</v>
       </c>
@@ -3023,18 +3412,19 @@
       <c r="E93" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F93" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F93" s="3"/>
       <c r="G93" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H93" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J93" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I93" s="3"/>
-    </row>
-    <row r="94" spans="1:9" ht="18">
+      <c r="K93" s="3"/>
+    </row>
+    <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>64</v>
       </c>
@@ -3050,20 +3440,24 @@
       <c r="E94" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F94" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F94" s="3"/>
       <c r="G94" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H94" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H94">
+        <v>23553</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J94" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I94" s="3" t="s">
+      <c r="K94" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="18">
+    <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>87</v>
       </c>
@@ -3075,16 +3469,22 @@
       <c r="E95" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F95" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3" t="s">
+      <c r="F95">
+        <v>1028</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95">
+        <v>199</v>
+      </c>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I95" s="3"/>
-    </row>
-    <row r="96" spans="1:9" ht="18">
+      <c r="K95" s="3"/>
+    </row>
+    <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>115</v>
       </c>
@@ -3098,12 +3498,13 @@
       </c>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
-      <c r="H96" s="3" t="s">
+      <c r="I96" s="3"/>
+      <c r="J96" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I96" s="3"/>
-    </row>
-    <row r="97" spans="1:9" ht="18">
+      <c r="K96" s="3"/>
+    </row>
+    <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>43</v>
       </c>
@@ -3115,18 +3516,21 @@
       <c r="E97" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3" t="s">
+      <c r="F97">
+        <v>507</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I97" s="3" t="s">
+      <c r="K97" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="18">
+    <row r="98" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>117</v>
       </c>
@@ -3140,12 +3544,13 @@
       </c>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
-      <c r="H98" s="3" t="s">
+      <c r="I98" s="3"/>
+      <c r="J98" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I98" s="3"/>
-    </row>
-    <row r="99" spans="1:9" ht="18">
+      <c r="K98" s="3"/>
+    </row>
+    <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>118</v>
       </c>
@@ -3157,18 +3562,24 @@
       <c r="E99" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>15</v>
+      <c r="F99" s="3">
+        <v>0</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H99" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H99">
+        <v>1118</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J99" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I99" s="3"/>
-    </row>
-    <row r="100" spans="1:9" ht="18">
+      <c r="K99" s="3"/>
+    </row>
+    <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>119</v>
       </c>
@@ -3180,18 +3591,24 @@
       <c r="E100" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F100" s="3" t="s">
-        <v>15</v>
+      <c r="F100">
+        <v>2</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H100" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H100">
+        <v>1126</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J100" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I100" s="3"/>
-    </row>
-    <row r="101" spans="1:9" ht="18">
+      <c r="K100" s="3"/>
+    </row>
+    <row r="101" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>142</v>
       </c>
@@ -3203,14 +3620,17 @@
       <c r="E101" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F101" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
+      <c r="F101">
+        <v>110383</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I101" s="3"/>
-    </row>
-    <row r="102" spans="1:9" ht="18">
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+    </row>
+    <row r="102" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>143</v>
       </c>
@@ -3226,16 +3646,22 @@
       <c r="E102" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F102" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="3" t="s">
+      <c r="F102">
+        <v>2597</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H102">
+        <v>5991</v>
+      </c>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="18">
+    <row r="103" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>144</v>
       </c>
@@ -3247,14 +3673,20 @@
       <c r="E103" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F103" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G103" s="3"/>
-      <c r="H103" s="3"/>
+      <c r="F103">
+        <v>1325</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H103">
+        <v>168497</v>
+      </c>
       <c r="I103" s="3"/>
-    </row>
-    <row r="104" spans="1:9" ht="18">
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+    </row>
+    <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>34</v>
       </c>
@@ -3266,18 +3698,24 @@
       <c r="E104" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F104" s="3" t="s">
-        <v>15</v>
+      <c r="F104">
+        <v>274</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H104" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H104">
+        <v>2768</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J104" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I104" s="3"/>
-    </row>
-    <row r="105" spans="1:9" ht="18">
+      <c r="K104" s="3"/>
+    </row>
+    <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>22</v>
       </c>
@@ -3291,18 +3729,24 @@
       <c r="E105" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F105" s="3" t="s">
-        <v>17</v>
+      <c r="F105">
+        <v>31</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H105" s="3" t="s">
+      <c r="H105">
+        <v>864</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J105" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I105" s="3"/>
-    </row>
-    <row r="106" spans="1:9" ht="18">
+      <c r="K105" s="3"/>
+    </row>
+    <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>23</v>
       </c>
@@ -3316,18 +3760,22 @@
       <c r="E106" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F106" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F106" s="3"/>
       <c r="G106" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H106" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H106">
+        <v>98</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J106" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I106" s="3"/>
-    </row>
-    <row r="107" spans="1:9" ht="18">
+      <c r="K106" s="3"/>
+    </row>
+    <row r="107" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>65</v>
       </c>
@@ -3341,20 +3789,21 @@
       <c r="E107" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F107" s="3"/>
       <c r="G107" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H107" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J107" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I107" s="3" t="s">
+      <c r="K107" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="18">
+    <row r="108" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>145</v>
       </c>
@@ -3366,16 +3815,22 @@
       <c r="E108" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F108" s="3" t="s">
-        <v>17</v>
+      <c r="F108">
+        <v>30035</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H108" s="3"/>
-      <c r="I108" s="3"/>
-    </row>
-    <row r="109" spans="1:9" ht="18">
+      <c r="H108">
+        <v>13809</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+    </row>
+    <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>167</v>
       </c>
@@ -3389,10 +3844,11 @@
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
       <c r="I109" s="3"/>
-    </row>
-    <row r="110" spans="1:9" ht="18">
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+    </row>
+    <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>51</v>
       </c>
@@ -3404,18 +3860,19 @@
       <c r="E110" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F110" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F110" s="3"/>
       <c r="G110" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H110" s="3" t="s">
+      <c r="I110" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J110" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I110" s="3"/>
-    </row>
-    <row r="111" spans="1:9" ht="18">
+      <c r="K110" s="3"/>
+    </row>
+    <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>88</v>
       </c>
@@ -3427,18 +3884,24 @@
       <c r="E111" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F111" s="3" t="s">
-        <v>17</v>
+      <c r="F111">
+        <v>6613</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H111" s="3" t="s">
+      <c r="H111">
+        <v>2949</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J111" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I111" s="3"/>
-    </row>
-    <row r="112" spans="1:9" ht="18">
+      <c r="K111" s="3"/>
+    </row>
+    <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>146</v>
       </c>
@@ -3450,16 +3913,19 @@
       <c r="E112" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F112" s="3" t="s">
-        <v>17</v>
+      <c r="F112">
+        <v>11633</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H112" s="3"/>
-      <c r="I112" s="3"/>
-    </row>
-    <row r="113" spans="1:9" ht="18">
+        <v>17</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+    </row>
+    <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>35</v>
       </c>
@@ -3469,18 +3935,24 @@
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
-      <c r="F113" s="3" t="s">
-        <v>17</v>
+      <c r="F113">
+        <v>534</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H113" s="3" t="s">
+      <c r="H113">
+        <v>7287</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J113" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I113" s="3"/>
-    </row>
-    <row r="114" spans="1:9" ht="18">
+      <c r="K113" s="3"/>
+    </row>
+    <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>89</v>
       </c>
@@ -3492,18 +3964,24 @@
       <c r="E114" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F114" s="3" t="s">
-        <v>17</v>
+      <c r="F114">
+        <v>8715</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H114" s="3" t="s">
+      <c r="H114">
+        <v>58</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J114" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I114" s="3"/>
-    </row>
-    <row r="115" spans="1:9" ht="18">
+      <c r="K114" s="3"/>
+    </row>
+    <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>44</v>
       </c>
@@ -3515,20 +3993,23 @@
       <c r="E115" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F115" s="3" t="s">
-        <v>17</v>
+      <c r="F115">
+        <v>12</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H115" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J115" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I115" s="3" t="s">
+      <c r="K115" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="18">
+    <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>130</v>
       </c>
@@ -3542,12 +4023,13 @@
       </c>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
-      <c r="H116" s="3" t="s">
+      <c r="I116" s="3"/>
+      <c r="J116" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I116" s="3"/>
-    </row>
-    <row r="117" spans="1:9" ht="18">
+      <c r="K116" s="3"/>
+    </row>
+    <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>147</v>
       </c>
@@ -3559,16 +4041,22 @@
       <c r="E117" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F117" s="3" t="s">
-        <v>17</v>
+      <c r="F117">
+        <v>312812</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H117" s="3"/>
-      <c r="I117" s="3"/>
-    </row>
-    <row r="118" spans="1:9" ht="18">
+      <c r="H117">
+        <v>52630</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J117" s="3"/>
+      <c r="K117" s="3"/>
+    </row>
+    <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>36</v>
       </c>
@@ -3580,18 +4068,18 @@
       <c r="E118" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F118" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="G118" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H118" s="3" t="s">
+      <c r="I118" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J118" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I118" s="3"/>
-    </row>
-    <row r="119" spans="1:9" ht="18">
+      <c r="K118" s="3"/>
+    </row>
+    <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>148</v>
       </c>
@@ -3603,16 +4091,22 @@
       <c r="E119" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F119" s="3" t="s">
-        <v>17</v>
+      <c r="F119">
+        <v>310490</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H119" s="3"/>
-      <c r="I119" s="3"/>
-    </row>
-    <row r="120" spans="1:9" ht="18">
+      <c r="H119">
+        <v>52601</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J119" s="3"/>
+      <c r="K119" s="3"/>
+    </row>
+    <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>149</v>
       </c>
@@ -3624,16 +4118,20 @@
       <c r="E120" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F120" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F120" s="3"/>
       <c r="G120" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H120" s="3"/>
-      <c r="I120" s="3"/>
-    </row>
-    <row r="121" spans="1:9" ht="18">
+        <v>15</v>
+      </c>
+      <c r="H120">
+        <v>35</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+    </row>
+    <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>150</v>
       </c>
@@ -3645,16 +4143,22 @@
       <c r="E121" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F121" s="3" t="s">
-        <v>17</v>
+      <c r="F121">
+        <v>75264</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H121" s="3"/>
-      <c r="I121" s="3"/>
-    </row>
-    <row r="122" spans="1:9" ht="18">
+      <c r="H121">
+        <v>16852</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+    </row>
+    <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>37</v>
       </c>
@@ -3666,18 +4170,22 @@
       <c r="E122" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F122" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F122" s="3"/>
       <c r="G122" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H122" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H122">
+        <v>13398</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J122" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I122" s="3"/>
-    </row>
-    <row r="123" spans="1:9" ht="18">
+      <c r="K122" s="3"/>
+    </row>
+    <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>66</v>
       </c>
@@ -3689,20 +4197,21 @@
       <c r="E123" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F123" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F123" s="3"/>
       <c r="G123" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H123" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J123" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I123" s="3" t="s">
+      <c r="K123" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="18">
+    <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>151</v>
       </c>
@@ -3714,16 +4223,22 @@
       <c r="E124" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F124" s="3" t="s">
-        <v>17</v>
+      <c r="F124">
+        <v>2044</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H124" s="3"/>
-      <c r="I124" s="3"/>
-    </row>
-    <row r="125" spans="1:9" ht="18">
+      <c r="H124">
+        <v>5843</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+    </row>
+    <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>152</v>
       </c>
@@ -3735,16 +4250,22 @@
       <c r="E125" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F125" s="3" t="s">
-        <v>17</v>
+      <c r="F125" s="3">
+        <v>2844</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H125" s="3"/>
-      <c r="I125" s="3"/>
-    </row>
-    <row r="126" spans="1:9" ht="18">
+      <c r="H125">
+        <v>1036</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J125" s="3"/>
+      <c r="K125" s="3"/>
+    </row>
+    <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>138</v>
       </c>
@@ -3757,15 +4278,16 @@
         <v>40</v>
       </c>
       <c r="F126" s="3"/>
-      <c r="G126" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H126" s="3" t="s">
+      <c r="G126" s="3"/>
+      <c r="I126" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J126" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I126" s="3"/>
-    </row>
-    <row r="127" spans="1:9" ht="18">
+      <c r="K126" s="3"/>
+    </row>
+    <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>47</v>
       </c>
@@ -3777,18 +4299,21 @@
       <c r="E127" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F127" s="3" t="s">
-        <v>17</v>
+      <c r="F127">
+        <v>51</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H127" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J127" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I127" s="3"/>
-    </row>
-    <row r="128" spans="1:9" ht="18">
+      <c r="K127" s="3"/>
+    </row>
+    <row r="128" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>154</v>
       </c>
@@ -3800,16 +4325,22 @@
       <c r="E128" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F128" s="3" t="s">
-        <v>17</v>
+      <c r="F128">
+        <v>3195</v>
       </c>
       <c r="G128" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H128" s="3"/>
-      <c r="I128" s="3"/>
-    </row>
-    <row r="129" spans="1:9" ht="18">
+      <c r="H128">
+        <v>1036</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+    </row>
+    <row r="129" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>140</v>
       </c>
@@ -3823,12 +4354,13 @@
       </c>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
-      <c r="H129" s="3" t="s">
+      <c r="I129" s="3"/>
+      <c r="J129" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I129" s="3"/>
-    </row>
-    <row r="130" spans="1:9" ht="18">
+      <c r="K129" s="3"/>
+    </row>
+    <row r="130" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>165</v>
       </c>
@@ -3840,12 +4372,13 @@
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
       <c r="G130" s="3"/>
-      <c r="H130" s="3"/>
-      <c r="I130" s="3" t="s">
+      <c r="I130" s="3"/>
+      <c r="J130" s="3"/>
+      <c r="K130" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="18">
+    <row r="131" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>155</v>
       </c>
@@ -3857,16 +4390,19 @@
       <c r="E131" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F131" s="3" t="s">
-        <v>17</v>
+      <c r="F131">
+        <v>265</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H131" s="3"/>
-      <c r="I131" s="3"/>
-    </row>
-    <row r="132" spans="1:9" ht="15" customHeight="1">
+      <c r="I131" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J131" s="3"/>
+      <c r="K131" s="3"/>
+    </row>
+    <row r="132" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>77</v>
       </c>
@@ -3878,18 +4414,24 @@
       <c r="E132" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F132" s="3" t="s">
-        <v>17</v>
+      <c r="F132">
+        <v>359</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H132" s="3" t="s">
+      <c r="H132">
+        <v>1352</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J132" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I132" s="3"/>
-    </row>
-    <row r="133" spans="1:9" s="3" customFormat="1" ht="18">
+      <c r="K132" s="3"/>
+    </row>
+    <row r="133" spans="1:11" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>79</v>
       </c>
@@ -3899,17 +4441,23 @@
       <c r="E133" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F133" s="3" t="s">
-        <v>17</v>
+      <c r="F133">
+        <v>467</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H133" s="3" t="s">
+      <c r="H133">
+        <v>2956</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J133" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="134" spans="1:9" s="3" customFormat="1" ht="18">
+    <row r="134" spans="1:11" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>141</v>
       </c>
@@ -3919,11 +4467,11 @@
       <c r="E134" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H134" s="3" t="s">
+      <c r="J134" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="135" spans="1:9" s="3" customFormat="1" ht="18">
+    <row r="135" spans="1:11" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>90</v>
       </c>
@@ -3935,17 +4483,23 @@
       <c r="E135" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F135" s="3" t="s">
-        <v>17</v>
+      <c r="F135">
+        <v>3850</v>
       </c>
       <c r="G135" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H135">
+        <v>502</v>
+      </c>
+      <c r="I135" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H135" s="3" t="s">
+      <c r="J135" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="136" spans="1:9" s="3" customFormat="1" ht="18">
+    <row r="136" spans="1:11" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>38</v>
       </c>
@@ -3957,17 +4511,20 @@
       <c r="E136" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F136" s="3" t="s">
-        <v>17</v>
+      <c r="F136">
+        <v>2658</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H136" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J136" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="137" spans="1:9" s="3" customFormat="1" ht="18">
+    <row r="137" spans="1:11" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>52</v>
       </c>
@@ -3981,17 +4538,20 @@
       <c r="E137" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F137" s="3" t="s">
-        <v>15</v>
+      <c r="F137" s="3">
+        <v>0</v>
       </c>
       <c r="G137" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H137" s="3" t="s">
+      <c r="I137" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J137" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="138" spans="1:9" s="3" customFormat="1" ht="18">
+    <row r="138" spans="1:11" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A138"/>
       <c r="B138"/>
       <c r="C138"/>
@@ -3999,8 +4559,31 @@
       <c r="E138"/>
       <c r="F138"/>
       <c r="G138"/>
-      <c r="H138"/>
       <c r="I138"/>
+      <c r="J138"/>
+      <c r="K138"/>
+    </row>
+    <row r="139" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F139">
+        <v>13</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A140" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F140">
+        <v>12</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A3:G134">

</xml_diff>

<commit_message>
add back publisher to list of allowed tags
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="I100" sqref="I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3577,7 +3577,7 @@
         <v>16</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="J99" s="3" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
added am and ex, update report, update ODD
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="14000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TESimplespreadsheet.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="177">
   <si>
     <t>code</t>
   </si>
@@ -524,9 +524,6 @@
     <t>do we need this?</t>
   </si>
   <si>
-    <t>do we need this</t>
-  </si>
-  <si>
     <t>handShift</t>
   </si>
   <si>
@@ -546,6 +543,15 @@
   </si>
   <si>
     <t>merge into empty ref</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>ex</t>
+  </si>
+  <si>
+    <t>table</t>
   </si>
 </sst>
 </file>
@@ -983,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K138"/>
+  <dimension ref="A1:K139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J93" sqref="J93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1011,13 +1017,13 @@
         <v>164</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>12</v>
@@ -1253,7 +1259,9 @@
       <c r="I10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="K10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1629,7 +1637,9 @@
       <c r="I24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J24" s="3"/>
+      <c r="J24" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="18">
@@ -1844,7 +1854,7 @@
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="18">
@@ -2581,7 +2591,7 @@
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="18">
@@ -2634,7 +2644,7 @@
     </row>
     <row r="63" spans="1:11" ht="18">
       <c r="A63" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4" t="s">
@@ -3073,7 +3083,7 @@
         <v>16</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="J80" s="3" t="s">
         <v>39</v>
@@ -3099,7 +3109,7 @@
         <v>16</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="J81" s="3" t="s">
         <v>39</v>
@@ -3130,7 +3140,9 @@
       <c r="I82" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J82" s="3"/>
+      <c r="J82" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="K82" s="3"/>
     </row>
     <row r="83" spans="1:11" ht="18">
@@ -3422,7 +3434,7 @@
         <v>16</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="J93" s="3" t="s">
         <v>39</v>
@@ -3532,7 +3544,7 @@
         <v>155</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="18">
@@ -3580,7 +3592,7 @@
         <v>97</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="K99" s="3"/>
     </row>
@@ -3609,7 +3621,7 @@
         <v>97</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="K100" s="3"/>
     </row>
@@ -3832,7 +3844,9 @@
       <c r="I108" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J108" s="3"/>
+      <c r="J108" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="K108" s="3"/>
     </row>
     <row r="109" spans="1:11" ht="18">
@@ -3849,7 +3863,9 @@
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
+      <c r="I109" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
     </row>
@@ -4240,7 +4256,9 @@
       <c r="I124" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J124" s="3"/>
+      <c r="J124" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="K124" s="3"/>
     </row>
     <row r="125" spans="1:11" ht="18">
@@ -4317,7 +4335,7 @@
         <v>155</v>
       </c>
       <c r="K127" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="18">
@@ -4382,7 +4400,7 @@
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
       <c r="K130" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:11" ht="18">
@@ -4559,16 +4577,33 @@
       </c>
     </row>
     <row r="138" spans="1:11" s="3" customFormat="1" ht="18">
-      <c r="A138"/>
+      <c r="A138" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="B138"/>
       <c r="C138"/>
       <c r="D138"/>
       <c r="E138"/>
       <c r="F138"/>
       <c r="H138"/>
-      <c r="I138"/>
-      <c r="J138"/>
+      <c r="I138" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J138" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="K138"/>
+    </row>
+    <row r="139" spans="1:11" ht="18">
+      <c r="A139" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J139" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A3:G134">

</xml_diff>

<commit_message>
add subst, make sure all elements are classified
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="200">
   <si>
     <t>code</t>
   </si>
   <si>
     <t>merge with milestone</t>
-  </si>
-  <si>
-    <t>merge into q?</t>
   </si>
   <si>
     <t>merge with hi</t>
@@ -488,9 +485,6 @@
     <t>group</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -615,13 +609,25 @@
   </si>
   <si>
     <t>editor</t>
+  </si>
+  <si>
+    <t>interpretation</t>
+  </si>
+  <si>
+    <t>merge into q</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>pictures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -675,6 +681,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -693,7 +705,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -715,8 +727,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -724,8 +754,9 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -736,6 +767,15 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -746,6 +786,15 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1082,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD159"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J114" sqref="J114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1097,42 +1146,42 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="J1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18">
       <c r="A2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -1143,23 +1192,25 @@
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="18">
       <c r="A3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1167,23 +1218,25 @@
         <v>16180</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>4470</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="18">
       <c r="A4" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="4">
         <v>55863</v>
@@ -1194,28 +1247,30 @@
         <v>7734</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>117</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K4" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="18">
       <c r="A5" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1223,28 +1278,28 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>1118</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="18">
       <c r="A6" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1252,28 +1307,28 @@
         <v>2</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>1126</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="18">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1281,24 +1336,24 @@
         <v>51</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="18">
       <c r="A8" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1309,122 +1364,124 @@
         <v>265</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>177</v>
+      </c>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="18">
       <c r="A9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="18">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="18">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="18">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="18">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="18">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="18">
       <c r="A16" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1432,30 +1489,30 @@
       <c r="F16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="18">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="18">
       <c r="A18" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1463,19 +1520,19 @@
       <c r="F18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" ht="18">
       <c r="A19" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1483,19 +1540,19 @@
       <c r="F19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" ht="18">
       <c r="A20" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1503,52 +1560,52 @@
       <c r="F20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="18">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="18">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="18">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="18">
       <c r="A24" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1558,30 +1615,30 @@
       <c r="F24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="18">
       <c r="A25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="18">
       <c r="A26" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1591,19 +1648,19 @@
       <c r="F26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" ht="18">
       <c r="A27" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1611,145 +1668,145 @@
       <c r="F27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" ht="18">
       <c r="A28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" ht="18">
       <c r="A29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="18">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="18">
       <c r="A31" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" ht="18">
       <c r="A32" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" ht="18">
       <c r="A33" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" ht="18">
       <c r="A34" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1757,19 +1814,19 @@
       <c r="F34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" ht="18">
       <c r="A35" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1777,52 +1834,52 @@
       <c r="F35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" ht="18">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="18">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="18">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="18">
       <c r="A39" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1830,52 +1887,52 @@
       <c r="F39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K39" s="3"/>
     </row>
     <row r="40" spans="1:11" ht="18">
       <c r="A40" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="H40" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11" ht="18">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="18">
       <c r="A42" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -1883,30 +1940,30 @@
       <c r="F42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" ht="18">
       <c r="A43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="18">
       <c r="A44" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1915,30 +1972,30 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:11" ht="18">
       <c r="A45" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="18">
       <c r="A46" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1946,25 +2003,25 @@
         <v>2844</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G46">
         <v>1036</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" ht="18">
       <c r="A47" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1972,44 +2029,44 @@
       <c r="F47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" ht="18">
       <c r="A48" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E48">
         <v>60496</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K48" s="3"/>
     </row>
     <row r="49" spans="1:11" ht="18">
       <c r="A49" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" s="4">
         <v>521192</v>
@@ -2020,28 +2077,28 @@
         <v>7015</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G49">
         <v>69</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K49" s="3"/>
     </row>
     <row r="50" spans="1:11" ht="18">
       <c r="A50" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -2049,25 +2106,25 @@
         <v>0</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G50">
         <v>12</v>
       </c>
       <c r="H50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J50" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:11" ht="18">
       <c r="A51" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51" s="4">
         <v>1809</v>
@@ -2078,128 +2135,132 @@
         <v>137</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K51" s="3"/>
     </row>
     <row r="52" spans="1:11" ht="18">
       <c r="A52" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K52" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="18">
       <c r="A53" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J53" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K53" s="3"/>
     </row>
     <row r="54" spans="1:11" ht="18">
       <c r="A54" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J54" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K54" s="3"/>
     </row>
     <row r="55" spans="1:11" ht="18">
       <c r="A55" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="18">
       <c r="A56" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G56" s="3"/>
       <c r="I56" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="18">
       <c r="A57" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -2208,18 +2269,20 @@
         <v>29</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J57" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K57" s="3"/>
     </row>
     <row r="58" spans="1:11" ht="18">
       <c r="A58" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" s="3">
         <v>60149</v>
@@ -2230,25 +2293,25 @@
         <v>1795</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G58">
         <v>3001</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K58" s="3"/>
     </row>
     <row r="59" spans="1:11" ht="18">
       <c r="A59" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59" s="4">
         <v>20843</v>
@@ -2259,25 +2322,25 @@
         <v>7734</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G59">
         <v>753</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K59" s="3"/>
     </row>
     <row r="60" spans="1:11" ht="18">
       <c r="A60" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B60" s="4">
         <v>89899</v>
@@ -2288,25 +2351,25 @@
         <v>9246</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G60">
         <v>1378</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K60" s="3"/>
     </row>
     <row r="61" spans="1:11" ht="18">
       <c r="A61" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="4">
         <v>10046</v>
@@ -2317,193 +2380,195 @@
         <v>3549</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G61">
         <v>1228</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K61" s="3"/>
     </row>
     <row r="62" spans="1:11" ht="18">
       <c r="A62" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="H62" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K62" s="3"/>
     </row>
     <row r="63" spans="1:11" ht="18">
       <c r="A63" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E63">
         <v>30299</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J63" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="K63" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="18">
       <c r="A64" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G64">
         <v>58</v>
       </c>
       <c r="H64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J64" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="K64" s="3"/>
     </row>
     <row r="65" spans="1:11" ht="18">
       <c r="A65" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E65">
         <v>90</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G65">
         <v>903</v>
       </c>
       <c r="H65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="K65" s="3"/>
     </row>
     <row r="66" spans="1:11" ht="18">
       <c r="A66" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E66">
         <v>4</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G66">
         <v>87</v>
       </c>
       <c r="H66" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="K66" s="3"/>
     </row>
     <row r="67" spans="1:11" ht="18">
       <c r="A67" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G67">
         <v>27874</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K67" s="3"/>
     </row>
     <row r="68" spans="1:11" ht="18">
       <c r="A68" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B68" s="4">
         <v>3478371</v>
@@ -2514,28 +2579,28 @@
         <v>138105</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G68">
         <v>37698</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K68" s="3"/>
     </row>
     <row r="69" spans="1:11" ht="18">
       <c r="A69" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -2543,28 +2608,28 @@
         <v>770</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G69">
         <v>10128</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K69" s="3"/>
     </row>
     <row r="70" spans="1:11" ht="18">
       <c r="A70" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -2572,23 +2637,25 @@
         <v>155</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G70">
         <v>5566</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J70" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K70" s="3"/>
     </row>
     <row r="71" spans="1:11" ht="18">
       <c r="A71" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" s="4">
         <v>102946</v>
@@ -2599,19 +2666,19 @@
         <v>9414</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G71">
         <v>1806</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K71" s="3"/>
     </row>
@@ -2626,23 +2693,25 @@
         <v>1</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J72" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="K72" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="18">
       <c r="A73" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -2650,53 +2719,53 @@
         <v>505</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G73">
         <v>7292</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K73" s="3"/>
     </row>
     <row r="74" spans="1:11" ht="18">
       <c r="A74" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J74" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K74" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="18">
       <c r="A75" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B75" s="4">
         <v>45062</v>
@@ -2707,28 +2776,28 @@
         <v>7247</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G75">
         <v>3641</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K75" s="3"/>
     </row>
     <row r="76" spans="1:11" ht="18">
       <c r="A76" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -2736,25 +2805,25 @@
         <v>15</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K76" s="3"/>
     </row>
     <row r="77" spans="1:11" ht="18">
       <c r="A77" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -2762,20 +2831,20 @@
         <v>125150</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K77" s="3"/>
     </row>
     <row r="78" spans="1:11" ht="18">
       <c r="A78" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B78" s="4">
         <v>1299500</v>
@@ -2786,28 +2855,28 @@
         <v>85352</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G78">
         <v>124593</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K78" s="3"/>
     </row>
     <row r="79" spans="1:11" ht="18">
       <c r="A79" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -2815,28 +2884,28 @@
         <v>381</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G79">
         <v>1021</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K79" s="3"/>
     </row>
     <row r="80" spans="1:11" ht="18">
       <c r="A80" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -2844,55 +2913,55 @@
         <v>6</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G80">
         <v>1105</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K80" s="3"/>
     </row>
     <row r="81" spans="1:11" ht="18">
       <c r="A81" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G81">
         <v>15</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K81" s="3"/>
     </row>
     <row r="82" spans="1:11" ht="18">
       <c r="A82" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -2900,28 +2969,28 @@
         <v>223</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G82">
         <v>1159</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K82" s="3"/>
     </row>
     <row r="83" spans="1:11" ht="18">
       <c r="A83" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -2929,25 +2998,25 @@
         <v>349</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G83">
         <v>1427</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K83" s="3"/>
     </row>
     <row r="84" spans="1:11" ht="18">
       <c r="A84" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -2956,20 +3025,22 @@
         <v>6711</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J84" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="K84" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="18">
       <c r="A85" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" s="4">
         <v>34583</v>
@@ -2980,63 +3051,63 @@
         <v>2645</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G85">
         <v>155</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K85" s="3"/>
     </row>
     <row r="86" spans="1:11" ht="18">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="18">
       <c r="A87" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G87">
         <v>69</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K87" s="3"/>
     </row>
     <row r="88" spans="1:11" ht="18">
       <c r="A88" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B88" s="4">
         <v>19247</v>
@@ -3047,23 +3118,25 @@
         <v>1147</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J88" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="K88" s="3"/>
     </row>
     <row r="89" spans="1:11" ht="18">
       <c r="A89" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -3071,59 +3144,59 @@
         <v>5247</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G89">
         <v>23175</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="K89" s="3"/>
     </row>
     <row r="90" spans="1:11" ht="18">
       <c r="A90" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B90" s="6">
         <v>34511</v>
       </c>
       <c r="C90" s="6"/>
       <c r="D90" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E90">
         <v>6120</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G90">
         <v>342</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K90" s="3"/>
     </row>
     <row r="91" spans="1:11" ht="18">
       <c r="A91" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
@@ -3131,76 +3204,80 @@
         <v>2365</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G91">
         <v>4462</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J91" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="K91" s="3"/>
     </row>
     <row r="92" spans="1:11" ht="18">
       <c r="A92" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K92" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K92" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="18">
       <c r="A93" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G93">
         <v>27014</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J93" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K93" s="3"/>
     </row>
     <row r="94" spans="1:11" ht="18">
       <c r="A94" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B94" s="4">
         <v>40756</v>
@@ -3211,85 +3288,87 @@
         <v>2815</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G94">
         <v>1040</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K94" s="3"/>
     </row>
     <row r="95" spans="1:11" ht="18">
       <c r="A95" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E95">
         <v>15</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G95">
         <v>402921</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K95" s="3"/>
     </row>
     <row r="96" spans="1:11" ht="18">
       <c r="A96" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E96">
         <v>489</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G96">
         <v>493</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J96" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="K96" s="3"/>
     </row>
     <row r="97" spans="1:11" ht="18">
       <c r="A97" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B97" s="4">
         <v>108894</v>
@@ -3300,84 +3379,86 @@
         <v>125202</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G97">
         <v>6363</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K97" s="3"/>
     </row>
     <row r="98" spans="1:11" ht="18">
       <c r="A98" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J98" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K98" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K98" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:11" ht="18">
       <c r="A99" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E99">
         <v>45</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J99" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J99" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="K99" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="18">
       <c r="A100" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
@@ -3385,20 +3466,22 @@
         <v>200</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J100" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="K100" s="3"/>
     </row>
     <row r="101" spans="1:11" ht="18">
       <c r="A101" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B101" s="4">
         <v>2311</v>
@@ -3409,29 +3492,29 @@
         <v>71</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K101" s="3"/>
     </row>
     <row r="102" spans="1:11" ht="18">
       <c r="A102" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E102" s="3">
         <v>0</v>
@@ -3439,16 +3522,16 @@
       <c r="F102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K102" s="3"/>
     </row>
     <row r="103" spans="1:11" ht="18">
       <c r="A103" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B103" s="4">
         <v>1541470</v>
@@ -3459,25 +3542,25 @@
         <v>115775</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G103">
         <v>144164</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K103" s="3"/>
     </row>
     <row r="104" spans="1:11" ht="18">
       <c r="A104" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B104" s="4">
         <v>46780581</v>
@@ -3488,26 +3571,28 @@
         <v>1419289</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G104">
         <v>2758132</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J104" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J104" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K104" s="3"/>
     </row>
     <row r="105" spans="1:11" ht="18">
       <c r="A105" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
@@ -3515,28 +3600,28 @@
         <v>23</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G105">
         <v>72</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K105" s="3"/>
     </row>
     <row r="106" spans="1:11" ht="18">
       <c r="A106" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
@@ -3544,23 +3629,25 @@
         <v>188278</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G106">
         <v>229168</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J106" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K106" s="3"/>
     </row>
     <row r="107" spans="1:11" ht="18">
       <c r="A107" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B107" s="4">
         <v>10272751</v>
@@ -3571,23 +3658,23 @@
         <v>1428379</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G107">
         <v>631256</v>
       </c>
       <c r="H107" s="3"/>
       <c r="I107" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K107" s="3"/>
     </row>
     <row r="108" spans="1:11" ht="18">
       <c r="A108" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B108" s="4">
         <v>185529</v>
@@ -3598,18 +3685,20 @@
         <v>19570</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J108" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K108" s="3"/>
     </row>
     <row r="109" spans="1:11" ht="18">
       <c r="A109" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B109" s="4">
         <v>22738</v>
@@ -3620,23 +3709,23 @@
         <v>1508235</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G109">
         <v>11923956</v>
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K109" s="3"/>
     </row>
     <row r="110" spans="1:11" ht="18">
       <c r="A110" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B110" s="4">
         <v>714182</v>
@@ -3647,23 +3736,23 @@
         <v>86396</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G110">
         <v>96717</v>
       </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K110" s="3"/>
     </row>
     <row r="111" spans="1:11" ht="18">
       <c r="A111" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B111" s="4">
         <v>319957</v>
@@ -3674,76 +3763,78 @@
         <v>17848</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G111">
         <v>28676</v>
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K111" s="3"/>
     </row>
     <row r="112" spans="1:11" ht="18">
       <c r="A112" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G112">
         <v>26</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J112" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K112" s="3"/>
     </row>
     <row r="113" spans="1:11" ht="18">
       <c r="A113" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C113" s="3"/>
       <c r="D113" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J113" s="3" t="s">
-        <v>155</v>
+        <v>14</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="K113" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="114" spans="1:11" ht="18">
       <c r="A114" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B114" s="4">
         <v>732115</v>
@@ -3754,26 +3845,28 @@
         <v>14639</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G114">
         <v>57816</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J114" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K114" s="3"/>
     </row>
     <row r="115" spans="1:11" ht="18">
       <c r="A115" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
@@ -3781,53 +3874,53 @@
         <v>2541</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G115">
         <v>3</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J115" s="3" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="K115" s="3"/>
     </row>
     <row r="116" spans="1:11" ht="18">
       <c r="A116" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J116" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K116" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K116" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="18">
       <c r="A117" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B117" s="4">
         <v>4091422</v>
@@ -3838,43 +3931,47 @@
         <v>113910</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G117">
         <v>214219</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J117" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K117" s="3"/>
     </row>
     <row r="118" spans="1:11" ht="18">
       <c r="A118" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J118" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J118" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K118" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="119" spans="1:11" ht="18">
       <c r="A119" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B119" s="4">
         <v>66501</v>
@@ -3885,56 +3982,56 @@
         <v>9727</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G119">
         <v>531</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K119" s="3"/>
     </row>
     <row r="120" spans="1:11" ht="18">
       <c r="A120" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E120" s="3"/>
       <c r="F120" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J120" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K120" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K120" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="121" spans="1:11" ht="18">
       <c r="A121" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
@@ -3942,25 +4039,25 @@
         <v>274</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G121">
         <v>2772</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K121" s="3"/>
     </row>
     <row r="122" spans="1:11" ht="18">
       <c r="A122" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B122" s="4">
         <v>9793935</v>
@@ -3971,21 +4068,23 @@
         <v>1099529</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G122">
         <v>736405</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J122" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J122" s="7" t="s">
+        <v>177</v>
+      </c>
       <c r="K122" s="3"/>
     </row>
     <row r="123" spans="1:11" ht="18">
       <c r="A123" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B123" s="4">
         <v>4482600</v>
@@ -3996,115 +4095,115 @@
         <v>362846</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G123">
         <v>383056</v>
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J123" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K123" s="3"/>
     </row>
     <row r="124" spans="1:11" ht="18">
       <c r="A124" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E124" s="3"/>
       <c r="F124" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J124" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K124" s="3"/>
     </row>
     <row r="125" spans="1:11" ht="18">
       <c r="A125" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E125" s="3"/>
       <c r="F125" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G125">
         <v>27489</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J125" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K125" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K125" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="18">
       <c r="A126" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E126" s="3"/>
       <c r="F126" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G126">
         <v>23553</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J126" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K126" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K126" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="18">
       <c r="A127" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B127" s="4">
         <v>5048</v>
@@ -4115,23 +4214,23 @@
         <v>1028</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G127">
         <v>199</v>
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J127" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K127" s="3"/>
     </row>
     <row r="128" spans="1:11" ht="18">
       <c r="A128" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B128" s="3">
         <v>634</v>
@@ -4142,22 +4241,22 @@
         <v>507</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J128" s="3" t="s">
-        <v>155</v>
+        <v>14</v>
+      </c>
+      <c r="J128" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="K128" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="129" spans="1:11" ht="18">
       <c r="A129" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B129" s="3">
         <v>108</v>
@@ -4168,49 +4267,53 @@
         <v>110383</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J129" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K129" s="3"/>
     </row>
     <row r="130" spans="1:11" ht="18">
       <c r="A130" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B130" s="4">
         <v>579010</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E130">
         <v>2597</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G130">
         <v>5991</v>
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J130" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J130" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K130" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:11" ht="18">
       <c r="A131" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B131" s="4">
         <v>3488</v>
@@ -4221,24 +4324,26 @@
         <v>1325</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G131">
         <v>168497</v>
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J131" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J131" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K131" s="3"/>
     </row>
     <row r="132" spans="1:11" ht="18">
       <c r="A132" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
@@ -4246,109 +4351,109 @@
         <v>274</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G132">
         <v>2768</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K132" s="3"/>
     </row>
     <row r="133" spans="1:11" ht="15" customHeight="1">
       <c r="A133" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C133" s="3"/>
       <c r="D133" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E133">
         <v>31</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G133">
         <v>864</v>
       </c>
       <c r="H133" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J133" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="I133" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J133" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="K133" s="3"/>
     </row>
     <row r="134" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A134" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G134">
         <v>98</v>
       </c>
       <c r="H134" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J134" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="I134" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J134" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A135" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G135"/>
       <c r="H135" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J135" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K135" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K135" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="136" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A136" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B136" s="4">
         <v>955765</v>
@@ -4359,61 +4464,64 @@
         <v>30035</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G136">
         <v>13809</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J136" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="137" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A137" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B137" s="4"/>
       <c r="C137" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G137"/>
       <c r="I137" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="J137" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="138" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A138" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G138"/>
       <c r="H138" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J138" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="139" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A139" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B139" s="4">
         <v>54216</v>
@@ -4424,24 +4532,24 @@
         <v>6613</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G139">
         <v>2949</v>
       </c>
       <c r="H139" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I139" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J139" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="140" spans="1:11" ht="18">
       <c r="A140" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B140" s="4">
         <v>506546</v>
@@ -4452,23 +4560,25 @@
         <v>11633</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I140" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J140" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J140" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K140" s="3"/>
     </row>
     <row r="141" spans="1:11" ht="18">
       <c r="A141" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
@@ -4476,25 +4586,25 @@
         <v>534</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G141">
         <v>7287</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I141" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J141" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K141" s="3"/>
     </row>
     <row r="142" spans="1:11" ht="18">
       <c r="A142" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B142" s="4">
         <v>90170</v>
@@ -4505,25 +4615,25 @@
         <v>8715</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G142">
         <v>58</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I142" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J142" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K142" s="3"/>
     </row>
     <row r="143" spans="1:11" ht="18">
       <c r="A143" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B143" s="3">
         <v>0</v>
@@ -4534,24 +4644,24 @@
         <v>12</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H143" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I143" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J143" s="3" t="s">
-        <v>155</v>
+        <v>14</v>
+      </c>
+      <c r="J143" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="K143" s="3" t="s">
-        <v>2</v>
+        <v>197</v>
       </c>
     </row>
     <row r="144" spans="1:11" ht="18">
       <c r="A144" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B144" s="4">
         <v>1479103</v>
@@ -4562,46 +4672,48 @@
         <v>312812</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G144">
         <v>52630</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I144" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J144" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K144" s="3"/>
     </row>
     <row r="145" spans="1:11" ht="18">
       <c r="A145" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
       <c r="F145" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H145" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K145" s="3"/>
     </row>
     <row r="146" spans="1:11" ht="18">
       <c r="A146" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B146" s="4">
         <v>1471913</v>
@@ -4612,48 +4724,52 @@
         <v>310490</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G146">
         <v>52601</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I146" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J146" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J146" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K146" s="3"/>
     </row>
     <row r="147" spans="1:11" ht="18">
       <c r="A147" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
       <c r="F147" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G147">
         <v>35</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I147" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J147" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K147" s="3"/>
     </row>
     <row r="148" spans="1:11" ht="18">
       <c r="A148" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B148" s="4">
         <v>220000</v>
@@ -4664,87 +4780,89 @@
         <v>75264</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G148">
         <v>16852</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J148" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="K148" s="3"/>
     </row>
     <row r="149" spans="1:11" ht="18">
       <c r="A149" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I149" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J149" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="18">
       <c r="A150" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
       <c r="F150" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G150">
         <v>13398</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J150" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K150" s="3"/>
     </row>
     <row r="151" spans="1:11" ht="18">
       <c r="A151" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
       <c r="F151" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J151" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K151" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K151" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="152" spans="1:11" ht="18">
       <c r="A152" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B152" s="4">
         <v>58531</v>
@@ -4755,25 +4873,25 @@
         <v>2044</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G152">
         <v>5843</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J152" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K152" s="3"/>
     </row>
     <row r="153" spans="1:11" ht="18">
       <c r="A153" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B153" s="4">
         <v>57697</v>
@@ -4784,48 +4902,50 @@
         <v>3195</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G153">
         <v>1036</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J153" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K153" s="3"/>
     </row>
     <row r="154" spans="1:11" ht="18">
       <c r="A154" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B154" s="5"/>
       <c r="C154" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D154" s="5"/>
       <c r="E154" s="3"/>
       <c r="F154" s="3"/>
       <c r="H154" s="3"/>
       <c r="I154" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J154" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J154" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="K154" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="155" spans="1:11" ht="18">
       <c r="A155" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
@@ -4833,28 +4953,28 @@
         <v>359</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G155">
         <v>1352</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J155" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K155" s="3"/>
     </row>
     <row r="156" spans="1:11" ht="18">
       <c r="A156" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
@@ -4862,25 +4982,25 @@
         <v>467</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G156">
         <v>2956</v>
       </c>
       <c r="H156" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J156" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K156" s="3"/>
     </row>
     <row r="157" spans="1:11" ht="18">
       <c r="A157" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B157" s="4">
         <v>58254</v>
@@ -4891,25 +5011,25 @@
         <v>3850</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G157">
         <v>502</v>
       </c>
       <c r="H157" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J157" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K157" s="3"/>
     </row>
     <row r="158" spans="1:11" ht="18">
       <c r="A158" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B158" s="4">
         <v>4022</v>
@@ -4920,46 +5040,46 @@
         <v>2658</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G158" s="3"/>
       <c r="H158" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J158" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K158" s="3"/>
     </row>
     <row r="159" spans="1:11" ht="18">
       <c r="A159" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C159" s="5"/>
       <c r="D159" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E159" s="3">
         <v>0</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G159" s="3"/>
       <c r="H159" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J159" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K159" s="3"/>
     </row>

</xml_diff>

<commit_message>
add rhyme element to mix
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="194">
   <si>
     <t>code</t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>typeDesc</t>
+  </si>
+  <si>
+    <t>rhyme</t>
   </si>
 </sst>
 </file>
@@ -1128,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K161"/>
+  <dimension ref="A1:K162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A32" sqref="A31:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I124" sqref="I124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4171,39 +4174,19 @@
       </c>
     </row>
     <row r="124" spans="1:11" ht="18">
-      <c r="A124" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124">
-        <v>31</v>
-      </c>
-      <c r="F124" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G124">
-        <v>864</v>
-      </c>
-      <c r="H124" s="3" t="s">
-        <v>11</v>
+      <c r="A124" t="s">
+        <v>193</v>
       </c>
       <c r="I124" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J124" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K124" s="3"/>
+        <v>182</v>
+      </c>
     </row>
     <row r="125" spans="1:11" ht="18">
       <c r="A125" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>9</v>
@@ -4212,12 +4195,14 @@
       <c r="D125" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E125" s="3"/>
+      <c r="E125">
+        <v>31</v>
+      </c>
       <c r="F125" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G125">
-        <v>98</v>
+        <v>864</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>11</v>
@@ -4232,7 +4217,7 @@
     </row>
     <row r="126" spans="1:11" ht="18">
       <c r="A126" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>9</v>
@@ -4245,6 +4230,9 @@
       <c r="F126" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G126">
+        <v>98</v>
+      </c>
       <c r="H126" s="3" t="s">
         <v>11</v>
       </c>
@@ -4252,29 +4240,24 @@
         <v>10</v>
       </c>
       <c r="J126" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K126" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="K126" s="3"/>
     </row>
     <row r="127" spans="1:11" ht="18">
       <c r="A127" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B127" s="4">
-        <v>955765</v>
-      </c>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4"/>
-      <c r="E127">
-        <v>30035</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127" s="3"/>
       <c r="F127" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G127">
-        <v>13809</v>
+        <v>9</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>11</v>
@@ -4283,154 +4266,157 @@
         <v>10</v>
       </c>
       <c r="J127" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K127" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="K127" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="128" spans="1:11" ht="18">
       <c r="A128" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B128" s="4"/>
-      <c r="C128" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
-      <c r="H128" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="B128" s="4">
+        <v>955765</v>
+      </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128">
+        <v>30035</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G128">
+        <v>13809</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="I128" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J128" s="7" t="s">
-        <v>182</v>
+      <c r="J128" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="K128" s="3"/>
     </row>
     <row r="129" spans="1:11" ht="18">
       <c r="A129" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="K129" s="3"/>
+    </row>
+    <row r="130" spans="1:11" ht="18">
+      <c r="A130" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B129" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
-      <c r="E129" s="3"/>
-      <c r="F129" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H129" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I129" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J129" s="3" t="s">
+      <c r="B130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J130" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K129" s="3"/>
-    </row>
-    <row r="130" spans="1:11" ht="15" customHeight="1">
-      <c r="A130" s="3" t="s">
+      <c r="K130" s="3"/>
+    </row>
+    <row r="131" spans="1:11" ht="15" customHeight="1">
+      <c r="A131" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B130" s="4">
+      <c r="B131" s="4">
         <v>54216</v>
-      </c>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4"/>
-      <c r="E130">
-        <v>6613</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G130">
-        <v>2949</v>
-      </c>
-      <c r="H130" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J130" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K130" s="3"/>
-    </row>
-    <row r="131" spans="1:11" s="3" customFormat="1" ht="18">
-      <c r="A131" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B131" s="4">
-        <v>506546</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131">
-        <v>11633</v>
+        <v>6613</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G131"/>
+      <c r="G131">
+        <v>2949</v>
+      </c>
       <c r="H131" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I131" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J131" s="7" t="s">
-        <v>182</v>
-      </c>
+      <c r="J131" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K131" s="3"/>
     </row>
     <row r="132" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A132" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B132" s="4">
+        <v>506546</v>
+      </c>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
       <c r="E132">
-        <v>534</v>
+        <v>11633</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G132">
-        <v>7287</v>
-      </c>
+      <c r="G132"/>
       <c r="H132" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I132" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J132" s="3" t="s">
-        <v>19</v>
+      <c r="J132" s="7" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A133" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B133" s="4">
-        <v>90170</v>
-      </c>
-      <c r="C133" s="4"/>
-      <c r="D133" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E133">
-        <v>8715</v>
+        <v>534</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G133">
-        <v>58</v>
+        <v>7287</v>
       </c>
       <c r="H133" s="3" t="s">
         <v>11</v>
@@ -4439,148 +4425,149 @@
         <v>10</v>
       </c>
       <c r="J133" s="3" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
     </row>
     <row r="134" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A134" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B134" s="3">
-        <v>0</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B134" s="4">
+        <v>90170</v>
+      </c>
+      <c r="C134" s="4"/>
+      <c r="D134" s="4"/>
       <c r="E134">
-        <v>12</v>
+        <v>8715</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G134"/>
+      <c r="G134">
+        <v>58</v>
+      </c>
       <c r="H134" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I134" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J134" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="K134" s="3" t="s">
-        <v>190</v>
+      <c r="J134" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="135" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A135" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C135" s="5"/>
-      <c r="D135" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B135" s="3">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>12</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G135"/>
+      <c r="H135" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="I135" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J135" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="J135" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="K135" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="136" spans="1:11" s="3" customFormat="1" ht="18">
       <c r="A136" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+      <c r="G136"/>
+      <c r="I136" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J136" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" s="3" customFormat="1" ht="18">
+      <c r="A137" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B136" s="4">
+      <c r="B137" s="4">
         <v>1479103</v>
       </c>
-      <c r="C136" s="4"/>
-      <c r="D136" s="4"/>
-      <c r="E136">
+      <c r="C137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137">
         <v>312812</v>
       </c>
-      <c r="F136" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G136">
+      <c r="F137" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G137">
         <v>52630</v>
       </c>
-      <c r="H136" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I136" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J136" s="3" t="s">
+      <c r="H137" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J137" s="3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" ht="18">
-      <c r="A137" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C137" s="3"/>
-      <c r="D137" s="3"/>
-      <c r="F137" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H137" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I137" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J137" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K137" s="3"/>
     </row>
     <row r="138" spans="1:11" ht="18">
       <c r="A138" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B138" s="4">
-        <v>1471913</v>
-      </c>
-      <c r="C138" s="4"/>
-      <c r="D138" s="4"/>
-      <c r="E138">
-        <v>310490</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
       <c r="F138" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G138">
-        <v>52601</v>
+        <v>9</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I138" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J138" s="3" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="K138" s="3"/>
     </row>
     <row r="139" spans="1:11" ht="18">
       <c r="A139" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C139" s="3"/>
-      <c r="D139" s="3"/>
-      <c r="E139" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="B139" s="4">
+        <v>1471913</v>
+      </c>
+      <c r="C139" s="4"/>
+      <c r="D139" s="4"/>
+      <c r="E139">
+        <v>310490</v>
+      </c>
       <c r="F139" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G139">
-        <v>35</v>
+        <v>52601</v>
       </c>
       <c r="H139" s="3" t="s">
         <v>11</v>
@@ -4595,21 +4582,19 @@
     </row>
     <row r="140" spans="1:11" ht="18">
       <c r="A140" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B140" s="4">
-        <v>220000</v>
-      </c>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
-      <c r="E140">
-        <v>75264</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
       <c r="F140" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G140">
-        <v>16852</v>
+        <v>35</v>
       </c>
       <c r="H140" s="3" t="s">
         <v>11</v>
@@ -4624,33 +4609,36 @@
     </row>
     <row r="141" spans="1:11" ht="18">
       <c r="A141" s="3" t="s">
-        <v>163</v>
+        <v>140</v>
+      </c>
+      <c r="B141" s="4">
+        <v>220000</v>
+      </c>
+      <c r="C141" s="4"/>
+      <c r="D141" s="4"/>
+      <c r="E141">
+        <v>75264</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G141">
+        <v>16852</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="I141" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J141" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="K141" s="3"/>
     </row>
     <row r="142" spans="1:11" ht="18">
       <c r="A142" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C142" s="3"/>
-      <c r="D142" s="3"/>
-      <c r="E142" s="3"/>
-      <c r="F142" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G142">
-        <v>13398</v>
-      </c>
-      <c r="H142" s="3" t="s">
-        <v>11</v>
+        <v>163</v>
       </c>
       <c r="I142" s="3" t="s">
         <v>10</v>
@@ -4658,11 +4646,10 @@
       <c r="J142" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K142" s="3"/>
     </row>
     <row r="143" spans="1:11" ht="18">
       <c r="A143" s="3" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>9</v>
@@ -4673,6 +4660,9 @@
       <c r="F143" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G143">
+        <v>13398</v>
+      </c>
       <c r="H143" s="3" t="s">
         <v>11</v>
       </c>
@@ -4680,29 +4670,22 @@
         <v>10</v>
       </c>
       <c r="J143" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K143" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="K143" s="3"/>
     </row>
     <row r="144" spans="1:11" ht="18">
       <c r="A144" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B144" s="4">
-        <v>58531</v>
-      </c>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
-      <c r="E144">
-        <v>2044</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
       <c r="F144" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G144">
-        <v>5843</v>
+        <v>9</v>
       </c>
       <c r="H144" s="3" t="s">
         <v>11</v>
@@ -4711,48 +4694,62 @@
         <v>10</v>
       </c>
       <c r="J144" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K144" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="K144" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="145" spans="1:11" ht="18">
       <c r="A145" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C145" s="3"/>
-      <c r="D145" s="3"/>
-      <c r="E145" s="3">
-        <v>2844</v>
+        <v>141</v>
+      </c>
+      <c r="B145" s="4">
+        <v>58531</v>
+      </c>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145">
+        <v>2044</v>
       </c>
       <c r="F145" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G145">
-        <v>1036</v>
+        <v>5843</v>
       </c>
       <c r="H145" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K145" s="3"/>
     </row>
     <row r="146" spans="1:11" ht="18">
       <c r="A146" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B146" s="4"/>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
-      <c r="F146" s="3"/>
-      <c r="H146" s="3"/>
+        <v>142</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3">
+        <v>2844</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G146">
+        <v>1036</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="I146" s="3" t="s">
         <v>143</v>
       </c>
@@ -4763,192 +4760,180 @@
     </row>
     <row r="147" spans="1:11" ht="18">
       <c r="A147" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B147" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C147" s="5"/>
-      <c r="D147" s="5"/>
-      <c r="E147" s="3"/>
+        <v>162</v>
+      </c>
+      <c r="B147" s="4"/>
+      <c r="C147" s="4"/>
+      <c r="D147" s="4"/>
       <c r="F147" s="3"/>
-      <c r="H147" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H147" s="3"/>
       <c r="I147" s="3" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="J147" s="3" t="s">
-        <v>34</v>
+        <v>164</v>
       </c>
       <c r="K147" s="3"/>
     </row>
     <row r="148" spans="1:11" ht="18">
       <c r="A148" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C148" s="3"/>
-      <c r="D148" s="3"/>
-      <c r="E148">
-        <v>51</v>
-      </c>
-      <c r="F148" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
       <c r="H148" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J148" s="3"/>
-      <c r="K148" s="3" t="s">
-        <v>136</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K148" s="3"/>
     </row>
     <row r="149" spans="1:11" ht="18">
       <c r="A149" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B149" s="4">
-        <v>57697</v>
-      </c>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
       <c r="E149">
-        <v>3195</v>
+        <v>51</v>
       </c>
       <c r="F149" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G149">
-        <v>1036</v>
-      </c>
       <c r="H149" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I149" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J149" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="K149" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="150" spans="1:11" ht="18">
       <c r="A150" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B150" s="4">
+        <v>57697</v>
+      </c>
+      <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150">
+        <v>3195</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G150">
+        <v>1036</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K150" s="3"/>
+    </row>
+    <row r="151" spans="1:11" ht="18">
+      <c r="A151" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B151" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C150" s="5"/>
-      <c r="D150" s="5"/>
-      <c r="E150" s="3"/>
-      <c r="F150" s="3"/>
-      <c r="H150" s="3"/>
-      <c r="I150" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J150" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K150" s="3"/>
-    </row>
-    <row r="151" spans="1:11" ht="18">
-      <c r="A151" t="s">
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="3"/>
+      <c r="H151" s="3"/>
+      <c r="I151" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J151" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K151" s="3"/>
+    </row>
+    <row r="152" spans="1:11" ht="18">
+      <c r="A152" t="s">
         <v>173</v>
       </c>
-      <c r="I151" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J151" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" ht="18">
-      <c r="A152" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B152" s="5"/>
-      <c r="C152" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D152" s="5"/>
-      <c r="E152" s="3"/>
-      <c r="F152" s="3"/>
-      <c r="H152" s="3"/>
       <c r="I152" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J152" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="K152" s="3" t="s">
-        <v>187</v>
+        <v>34</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="153" spans="1:11" ht="18">
       <c r="A153" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B153" s="3">
-        <v>0</v>
-      </c>
-      <c r="C153" s="3"/>
-      <c r="D153" s="3"/>
-      <c r="E153">
-        <v>265</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H153" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="B153" s="5"/>
+      <c r="C153" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" s="5"/>
+      <c r="E153" s="3"/>
+      <c r="F153" s="3"/>
+      <c r="H153" s="3"/>
       <c r="I153" s="3" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J153" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="K153" s="3"/>
+        <v>182</v>
+      </c>
+      <c r="K153" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="154" spans="1:11" ht="18">
       <c r="A154" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>9</v>
+        <v>145</v>
+      </c>
+      <c r="B154" s="3">
+        <v>0</v>
       </c>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154">
-        <v>359</v>
+        <v>265</v>
       </c>
       <c r="F154" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G154">
-        <v>1352</v>
-      </c>
       <c r="H154" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I154" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J154" s="3" t="s">
-        <v>60</v>
+        <v>90</v>
+      </c>
+      <c r="J154" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="K154" s="3"/>
     </row>
     <row r="155" spans="1:11" ht="18">
       <c r="A155" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>9</v>
@@ -4956,13 +4941,13 @@
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155">
-        <v>467</v>
+        <v>359</v>
       </c>
       <c r="F155" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G155">
-        <v>2956</v>
+        <v>1352</v>
       </c>
       <c r="H155" s="3" t="s">
         <v>11</v>
@@ -4977,131 +4962,160 @@
     </row>
     <row r="156" spans="1:11" ht="18">
       <c r="A156" s="3" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
-      <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
-      <c r="G156" s="3"/>
-      <c r="H156" s="3"/>
+      <c r="E156">
+        <v>467</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G156">
+        <v>2956</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="I156" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="J156" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K156" s="3"/>
     </row>
     <row r="157" spans="1:11" ht="18">
       <c r="A157" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3"/>
+      <c r="H157" s="3"/>
+      <c r="I157" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J157" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K157" s="3"/>
+    </row>
+    <row r="158" spans="1:11" ht="18">
+      <c r="A158" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B157" s="4">
+      <c r="B158" s="4">
         <v>58254</v>
       </c>
-      <c r="C157" s="4"/>
-      <c r="D157" s="4"/>
-      <c r="E157">
+      <c r="C158" s="4"/>
+      <c r="D158" s="4"/>
+      <c r="E158">
         <v>3850</v>
       </c>
-      <c r="F157" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G157">
+      <c r="F158" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G158">
         <v>502</v>
       </c>
-      <c r="H157" s="3" t="s">
+      <c r="H158" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I157" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J157" s="3" t="s">
+      <c r="I158" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J158" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K157" s="3"/>
-    </row>
-    <row r="158" spans="1:11" ht="18">
-      <c r="A158" t="s">
+      <c r="K158" s="3"/>
+    </row>
+    <row r="159" spans="1:11" ht="18">
+      <c r="A159" t="s">
         <v>192</v>
       </c>
-      <c r="I158" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J158" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" ht="18">
-      <c r="A159" s="3" t="s">
+      <c r="I159" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J159" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" ht="18">
+      <c r="A160" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B159" s="4">
+      <c r="B160" s="4">
         <v>4022</v>
       </c>
-      <c r="C159" s="4"/>
-      <c r="D159" s="4"/>
-      <c r="E159">
+      <c r="C160" s="4"/>
+      <c r="D160" s="4"/>
+      <c r="E160">
         <v>2658</v>
       </c>
-      <c r="F159" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G159" s="3"/>
-      <c r="H159" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I159" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J159" s="3" t="s">
+      <c r="F160" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G160" s="3"/>
+      <c r="H160" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I160" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J160" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K159" s="3"/>
-    </row>
-    <row r="160" spans="1:11" ht="18">
-      <c r="A160" t="s">
+      <c r="K160" s="3"/>
+    </row>
+    <row r="161" spans="1:11" ht="18">
+      <c r="A161" t="s">
         <v>176</v>
       </c>
-      <c r="I160" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J160" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11" ht="18">
-      <c r="A161" s="3" t="s">
+      <c r="I161" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J161" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" ht="18">
+      <c r="A162" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B161" s="5" t="s">
+      <c r="B162" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C161" s="5"/>
-      <c r="D161" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E161" s="3">
+      <c r="C162" s="5"/>
+      <c r="D162" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E162" s="3">
         <v>0</v>
       </c>
-      <c r="F161" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G161" s="3"/>
-      <c r="H161" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I161" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J161" s="3" t="s">
+      <c r="F162" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G162" s="3"/>
+      <c r="H162" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I162" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J162" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K161" s="3"/>
+      <c r="K162" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A3:K169">

</xml_diff>

<commit_message>
deal with #16, #17, #19, #20; rethinking list of headeronly elements is done; fixed Schematron check of headeronly so that it works
</commit_message>
<xml_diff>
--- a/TEISimplespreadsheet.xlsx
+++ b/TEISimplespreadsheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="197">
   <si>
     <t>code</t>
   </si>
@@ -603,6 +603,15 @@
   </si>
   <si>
     <t>rhyme</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>person</t>
   </si>
 </sst>
 </file>
@@ -694,8 +703,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -752,7 +765,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -775,6 +788,8 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -797,6 +812,8 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1131,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K162"/>
+  <dimension ref="A1:K165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I124" sqref="I124"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146:XFD146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1573,23 +1590,15 @@
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="18">
-      <c r="A18" s="8" t="s">
+      <c r="A18" t="s">
         <v>185</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K18" s="8"/>
+      <c r="I18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="18">
       <c r="A19" t="s">
@@ -3806,35 +3815,25 @@
     </row>
     <row r="108" spans="1:11" ht="18">
       <c r="A108" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K108" s="3"/>
+    </row>
+    <row r="109" spans="1:11" ht="15" customHeight="1">
+      <c r="A109" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H108" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I108" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J108" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K108" s="3"/>
-    </row>
-    <row r="109" spans="1:11" ht="18">
-      <c r="A109" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>9</v>
@@ -3849,161 +3848,149 @@
       <c r="F109" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G109">
+      <c r="H109" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J109" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K109" s="3"/>
+    </row>
+    <row r="110" spans="1:11" s="3" customFormat="1" ht="18">
+      <c r="A110" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110">
         <v>23553</v>
       </c>
-      <c r="H109" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I109" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J109" s="3" t="s">
+      <c r="H110" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K109" s="3" t="s">
+      <c r="K110" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="18">
-      <c r="A110" s="3" t="s">
+    <row r="111" spans="1:11" s="3" customFormat="1" ht="18">
+      <c r="A111" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B110" s="4">
+      <c r="B111" s="4">
         <v>5048</v>
       </c>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110">
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111">
         <v>1028</v>
       </c>
-      <c r="F110" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G110">
+      <c r="F111" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G111">
         <v>199</v>
       </c>
-      <c r="H110" s="3"/>
-      <c r="I110" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J110" s="3" t="s">
+      <c r="I111" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K110" s="3"/>
-    </row>
-    <row r="111" spans="1:11" ht="18">
-      <c r="A111" s="3" t="s">
+    </row>
+    <row r="112" spans="1:11" s="3" customFormat="1" ht="18">
+      <c r="A112" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B112" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="3"/>
-      <c r="F111" s="3"/>
-      <c r="H111" s="3"/>
-      <c r="I111" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J111" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K111" s="3"/>
-    </row>
-    <row r="112" spans="1:11" ht="18">
-      <c r="A112" s="3" t="s">
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="G112"/>
+      <c r="I112" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" s="3" customFormat="1" ht="18">
+      <c r="A113" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B113" s="3">
         <v>634</v>
       </c>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-      <c r="E112">
+      <c r="E113">
         <v>507</v>
       </c>
-      <c r="F112" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H112" s="3"/>
-      <c r="I112" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J112" s="7" t="s">
+      <c r="F113" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113"/>
+      <c r="I113" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="K112" s="3" t="s">
+      <c r="K113" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="18">
-      <c r="A113" s="3" t="s">
+    <row r="114" spans="1:11" s="3" customFormat="1" ht="18">
+      <c r="A114" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B114" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J113" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K113" s="3"/>
-    </row>
-    <row r="114" spans="1:11" ht="18">
-      <c r="A114" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3">
-        <v>0</v>
-      </c>
-      <c r="F114" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G114">
-        <v>1118</v>
-      </c>
-      <c r="H114" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="G114"/>
       <c r="I114" s="3" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K114" s="3"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="115" spans="1:11" ht="18">
       <c r="A115" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
-      <c r="E115">
-        <v>2</v>
+      <c r="E115" s="3">
+        <v>0</v>
       </c>
       <c r="F115" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G115">
-        <v>1126</v>
+        <v>1118</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>11</v>
@@ -4018,49 +4005,47 @@
     </row>
     <row r="116" spans="1:11" ht="18">
       <c r="A116" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B116" s="3">
-        <v>108</v>
+        <v>111</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116">
-        <v>110383</v>
+        <v>2</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H116" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="G116">
+        <v>1126</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="I116" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J116" s="7" t="s">
-        <v>182</v>
+        <v>90</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="K116" s="3"/>
     </row>
     <row r="117" spans="1:11" ht="18">
       <c r="A117" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B117" s="4">
-        <v>579010</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="B117" s="3">
+        <v>108</v>
+      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
       <c r="E117">
-        <v>2597</v>
+        <v>110383</v>
       </c>
       <c r="F117" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="G117">
-        <v>5991</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3" t="s">
@@ -4069,27 +4054,29 @@
       <c r="J117" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="K117" s="3" t="s">
-        <v>187</v>
-      </c>
+      <c r="K117" s="3"/>
     </row>
     <row r="118" spans="1:11" ht="18">
       <c r="A118" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B118" s="4">
-        <v>3488</v>
-      </c>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4"/>
+        <v>579010</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="E118">
-        <v>1325</v>
+        <v>2597</v>
       </c>
       <c r="F118" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G118">
-        <v>168497</v>
+        <v>5991</v>
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3" t="s">
@@ -4098,51 +4085,69 @@
       <c r="J118" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="K118" s="3"/>
+      <c r="K118" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="119" spans="1:11" ht="18">
       <c r="A119" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B119" s="4">
+        <v>3488</v>
+      </c>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119">
+        <v>1325</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G119">
+        <v>168497</v>
+      </c>
+      <c r="H119" s="3"/>
+      <c r="I119" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="K119" s="3"/>
+    </row>
+    <row r="120" spans="1:11" ht="18">
+      <c r="A120" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B119" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119">
+      <c r="B120" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120">
         <v>274</v>
       </c>
-      <c r="F119" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G119">
+      <c r="F120" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G120">
         <v>2768</v>
       </c>
-      <c r="H119" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I119" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J119" s="3" t="s">
+      <c r="H120" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J120" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K119" s="3"/>
-    </row>
-    <row r="120" spans="1:11" ht="18">
-      <c r="A120" t="s">
-        <v>170</v>
-      </c>
-      <c r="I120" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J120" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="K120" s="3"/>
     </row>
     <row r="121" spans="1:11" ht="18">
       <c r="A121" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="I121" s="3" t="s">
         <v>34</v>
@@ -4153,7 +4158,7 @@
     </row>
     <row r="122" spans="1:11" ht="18">
       <c r="A122" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="I122" s="3" t="s">
         <v>34</v>
@@ -4164,7 +4169,7 @@
     </row>
     <row r="123" spans="1:11" ht="18">
       <c r="A123" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I123" s="3" t="s">
         <v>34</v>
@@ -4175,49 +4180,29 @@
     </row>
     <row r="124" spans="1:11" ht="18">
       <c r="A124" t="s">
+        <v>172</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="18">
+      <c r="A125" t="s">
         <v>193</v>
       </c>
-      <c r="I124" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J124" s="3" t="s">
+      <c r="I125" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J125" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" ht="18">
-      <c r="A125" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125">
-        <v>31</v>
-      </c>
-      <c r="F125" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G125">
-        <v>864</v>
-      </c>
-      <c r="H125" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I125" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J125" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K125" s="3"/>
     </row>
     <row r="126" spans="1:11" ht="18">
       <c r="A126" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>9</v>
@@ -4226,12 +4211,14 @@
       <c r="D126" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E126" s="3"/>
+      <c r="E126">
+        <v>31</v>
+      </c>
       <c r="F126" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G126">
-        <v>98</v>
+        <v>864</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>11</v>
@@ -4246,7 +4233,7 @@
     </row>
     <row r="127" spans="1:11" ht="18">
       <c r="A127" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>9</v>
@@ -4259,6 +4246,9 @@
       <c r="F127" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G127">
+        <v>98</v>
+      </c>
       <c r="H127" s="3" t="s">
         <v>11</v>
       </c>
@@ -4266,29 +4256,24 @@
         <v>10</v>
       </c>
       <c r="J127" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K127" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="K127" s="3"/>
     </row>
     <row r="128" spans="1:11" ht="18">
       <c r="A128" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B128" s="4">
-        <v>955765</v>
-      </c>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4"/>
-      <c r="E128">
-        <v>30035</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" s="3"/>
       <c r="F128" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G128">
-        <v>13809</v>
+        <v>9</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>11</v>
@@ -4297,304 +4282,317 @@
         <v>10</v>
       </c>
       <c r="J128" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K128" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="129" spans="1:11" ht="18">
       <c r="A129" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B129" s="4"/>
-      <c r="C129" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D129" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E129" s="3"/>
-      <c r="F129" s="3"/>
-      <c r="H129" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="B129" s="4">
+        <v>955765</v>
+      </c>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129">
+        <v>30035</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G129">
+        <v>13809</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="I129" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J129" s="7" t="s">
-        <v>182</v>
+      <c r="J129" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="K129" s="3"/>
     </row>
     <row r="130" spans="1:11" ht="18">
       <c r="A130" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3"/>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J130" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="K130" s="3"/>
+    </row>
+    <row r="131" spans="1:11" ht="18">
+      <c r="A131" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B130" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
-      <c r="E130" s="3"/>
-      <c r="F130" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H130" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J130" s="3" t="s">
+      <c r="B131" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H131" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J131" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K130" s="3"/>
-    </row>
-    <row r="131" spans="1:11" ht="15" customHeight="1">
-      <c r="A131" s="3" t="s">
+      <c r="K131" s="3"/>
+    </row>
+    <row r="132" spans="1:11" ht="18">
+      <c r="A132" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B131" s="4">
+      <c r="B132" s="4">
         <v>54216</v>
-      </c>
-      <c r="C131" s="4"/>
-      <c r="D131" s="4"/>
-      <c r="E131">
-        <v>6613</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G131">
-        <v>2949</v>
-      </c>
-      <c r="H131" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I131" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J131" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K131" s="3"/>
-    </row>
-    <row r="132" spans="1:11" s="3" customFormat="1" ht="18">
-      <c r="A132" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B132" s="4">
-        <v>506546</v>
       </c>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132">
+        <v>6613</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G132">
+        <v>2949</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K132" s="3"/>
+    </row>
+    <row r="133" spans="1:11" ht="18">
+      <c r="A133" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B133" s="4">
+        <v>506546</v>
+      </c>
+      <c r="C133" s="4"/>
+      <c r="D133" s="4"/>
+      <c r="E133">
         <v>11633</v>
       </c>
-      <c r="F132" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G132"/>
-      <c r="H132" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I132" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J132" s="7" t="s">
+      <c r="F133" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J133" s="7" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" s="3" customFormat="1" ht="18">
-      <c r="A133" s="3" t="s">
+      <c r="K133" s="3"/>
+    </row>
+    <row r="134" spans="1:11" ht="18">
+      <c r="A134" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B133" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E133">
+      <c r="B134" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134">
         <v>534</v>
       </c>
-      <c r="F133" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G133">
+      <c r="F134" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G134">
         <v>7287</v>
       </c>
-      <c r="H133" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I133" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J133" s="3" t="s">
+      <c r="H134" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J134" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" s="3" customFormat="1" ht="18">
-      <c r="A134" s="3" t="s">
+      <c r="K134" s="3"/>
+    </row>
+    <row r="135" spans="1:11" ht="18">
+      <c r="A135" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B134" s="4">
+      <c r="B135" s="4">
         <v>90170</v>
       </c>
-      <c r="C134" s="4"/>
-      <c r="D134" s="4"/>
-      <c r="E134">
+      <c r="C135" s="4"/>
+      <c r="D135" s="4"/>
+      <c r="E135">
         <v>8715</v>
       </c>
-      <c r="F134" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G134">
+      <c r="F135" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G135">
         <v>58</v>
       </c>
-      <c r="H134" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I134" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J134" s="3" t="s">
+      <c r="H135" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J135" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" s="3" customFormat="1" ht="18">
-      <c r="A135" s="3" t="s">
+      <c r="K135" s="3"/>
+    </row>
+    <row r="136" spans="1:11" ht="18">
+      <c r="A136" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B135" s="3">
+      <c r="B136" s="3">
         <v>0</v>
       </c>
-      <c r="E135">
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136">
         <v>12</v>
       </c>
-      <c r="F135" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G135"/>
-      <c r="H135" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I135" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J135" s="7" t="s">
+      <c r="F136" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J136" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="K135" s="3" t="s">
+      <c r="K136" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="136" spans="1:11" s="3" customFormat="1" ht="18">
-      <c r="A136" s="3" t="s">
+    <row r="137" spans="1:11" ht="18">
+      <c r="A137" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B136" s="5" t="s">
+      <c r="B137" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C136" s="5"/>
-      <c r="D136" s="5"/>
-      <c r="G136"/>
-      <c r="I136" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J136" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" s="3" customFormat="1" ht="18">
-      <c r="A137" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B137" s="4">
-        <v>1479103</v>
-      </c>
-      <c r="C137" s="4"/>
-      <c r="D137" s="4"/>
-      <c r="E137">
-        <v>312812</v>
-      </c>
-      <c r="F137" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G137">
-        <v>52630</v>
-      </c>
-      <c r="H137" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="H137" s="3"/>
       <c r="I137" s="3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="J137" s="3" t="s">
-        <v>164</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="K137" s="3"/>
     </row>
     <row r="138" spans="1:11" ht="18">
       <c r="A138" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C138" s="3"/>
-      <c r="D138" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="B138" s="4">
+        <v>1479103</v>
+      </c>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138">
+        <v>312812</v>
+      </c>
       <c r="F138" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="G138">
+        <v>52630</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I138" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J138" s="3" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="K138" s="3"/>
     </row>
     <row r="139" spans="1:11" ht="18">
       <c r="A139" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B139" s="4">
-        <v>1471913</v>
-      </c>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
-      <c r="E139">
-        <v>310490</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
       <c r="F139" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G139">
-        <v>52601</v>
+        <v>9</v>
       </c>
       <c r="H139" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I139" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J139" s="3" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="K139" s="3"/>
     </row>
     <row r="140" spans="1:11" ht="18">
       <c r="A140" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C140" s="3"/>
-      <c r="D140" s="3"/>
-      <c r="E140" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="B140" s="4">
+        <v>1471913</v>
+      </c>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="E140">
+        <v>310490</v>
+      </c>
       <c r="F140" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G140">
-        <v>35</v>
+        <v>52601</v>
       </c>
       <c r="H140" s="3" t="s">
         <v>11</v>
@@ -4609,21 +4607,19 @@
     </row>
     <row r="141" spans="1:11" ht="18">
       <c r="A141" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B141" s="4">
-        <v>220000</v>
-      </c>
-      <c r="C141" s="4"/>
-      <c r="D141" s="4"/>
-      <c r="E141">
-        <v>75264</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
       <c r="F141" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G141">
-        <v>16852</v>
+        <v>35</v>
       </c>
       <c r="H141" s="3" t="s">
         <v>11</v>
@@ -4638,33 +4634,36 @@
     </row>
     <row r="142" spans="1:11" ht="18">
       <c r="A142" s="3" t="s">
-        <v>163</v>
+        <v>140</v>
+      </c>
+      <c r="B142" s="4">
+        <v>220000</v>
+      </c>
+      <c r="C142" s="4"/>
+      <c r="D142" s="4"/>
+      <c r="E142">
+        <v>75264</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G142">
+        <v>16852</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="I142" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J142" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="K142" s="3"/>
     </row>
     <row r="143" spans="1:11" ht="18">
       <c r="A143" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C143" s="3"/>
-      <c r="D143" s="3"/>
-      <c r="E143" s="3"/>
-      <c r="F143" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G143">
-        <v>13398</v>
-      </c>
-      <c r="H143" s="3" t="s">
-        <v>11</v>
+        <v>163</v>
       </c>
       <c r="I143" s="3" t="s">
         <v>10</v>
@@ -4672,11 +4671,10 @@
       <c r="J143" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K143" s="3"/>
     </row>
     <row r="144" spans="1:11" ht="18">
       <c r="A144" s="3" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>9</v>
@@ -4687,6 +4685,9 @@
       <c r="F144" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G144">
+        <v>13398</v>
+      </c>
       <c r="H144" s="3" t="s">
         <v>11</v>
       </c>
@@ -4694,29 +4695,22 @@
         <v>10</v>
       </c>
       <c r="J144" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K144" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="K144" s="3"/>
     </row>
     <row r="145" spans="1:11" ht="18">
       <c r="A145" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B145" s="4">
-        <v>58531</v>
-      </c>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
-      <c r="E145">
-        <v>2044</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
       <c r="F145" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G145">
-        <v>5843</v>
+        <v>9</v>
       </c>
       <c r="H145" s="3" t="s">
         <v>11</v>
@@ -4725,361 +4719,374 @@
         <v>10</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K145" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="K145" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="146" spans="1:11" ht="18">
       <c r="A146" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C146" s="3"/>
-      <c r="D146" s="3"/>
-      <c r="E146" s="3">
-        <v>2844</v>
+        <v>141</v>
+      </c>
+      <c r="B146" s="4">
+        <v>58531</v>
+      </c>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
+      <c r="E146">
+        <v>2044</v>
       </c>
       <c r="F146" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G146">
-        <v>1036</v>
+        <v>5843</v>
       </c>
       <c r="H146" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I146" s="3" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="J146" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K146" s="3"/>
     </row>
     <row r="147" spans="1:11" ht="18">
       <c r="A147" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B147" s="4"/>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+        <v>195</v>
+      </c>
+      <c r="B147" s="3"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3"/>
+      <c r="E147" s="3"/>
       <c r="F147" s="3"/>
       <c r="H147" s="3"/>
       <c r="I147" s="3" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="J147" s="3" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="K147" s="3"/>
     </row>
     <row r="148" spans="1:11" ht="18">
       <c r="A148" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B148" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C148" s="5"/>
-      <c r="D148" s="5"/>
-      <c r="E148" s="3"/>
-      <c r="F148" s="3"/>
+        <v>142</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3">
+        <v>2844</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G148">
+        <v>1036</v>
+      </c>
       <c r="H148" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="J148" s="3" t="s">
-        <v>34</v>
+        <v>164</v>
       </c>
       <c r="K148" s="3"/>
     </row>
     <row r="149" spans="1:11" ht="18">
       <c r="A149" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C149" s="3"/>
-      <c r="D149" s="3"/>
-      <c r="E149">
-        <v>51</v>
-      </c>
-      <c r="F149" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H149" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="4"/>
+      <c r="F149" s="3"/>
+      <c r="H149" s="3"/>
       <c r="I149" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J149" s="3"/>
-      <c r="K149" s="3" t="s">
-        <v>136</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K149" s="3"/>
     </row>
     <row r="150" spans="1:11" ht="18">
       <c r="A150" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B150" s="4">
-        <v>57697</v>
-      </c>
-      <c r="C150" s="4"/>
-      <c r="D150" s="4"/>
-      <c r="E150">
-        <v>3195</v>
-      </c>
-      <c r="F150" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G150">
-        <v>1036</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
       <c r="H150" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="J150" s="3" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="K150" s="3"/>
     </row>
     <row r="151" spans="1:11" ht="18">
       <c r="A151" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B151" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C151" s="5"/>
-      <c r="D151" s="5"/>
-      <c r="E151" s="3"/>
-      <c r="F151" s="3"/>
-      <c r="H151" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
+      <c r="E151">
+        <v>51</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="I151" s="3" t="s">
         <v>34</v>
       </c>
       <c r="J151" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K151" s="3"/>
+      <c r="K151" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="152" spans="1:11" ht="18">
-      <c r="A152" t="s">
-        <v>173</v>
+      <c r="A152" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B152" s="4">
+        <v>57697</v>
+      </c>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152">
+        <v>3195</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G152">
+        <v>1036</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="J152" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="K152" s="3"/>
     </row>
     <row r="153" spans="1:11" ht="18">
       <c r="A153" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B153" s="5"/>
-      <c r="C153" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" s="5"/>
       <c r="D153" s="5"/>
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
       <c r="H153" s="3"/>
       <c r="I153" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J153" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="K153" s="3" t="s">
-        <v>187</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K153" s="3"/>
     </row>
     <row r="154" spans="1:11" ht="18">
-      <c r="A154" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B154" s="3">
-        <v>0</v>
-      </c>
-      <c r="C154" s="3"/>
-      <c r="D154" s="3"/>
-      <c r="E154">
-        <v>265</v>
-      </c>
-      <c r="F154" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H154" s="3" t="s">
-        <v>11</v>
+      <c r="A154" t="s">
+        <v>173</v>
       </c>
       <c r="I154" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J154" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="K154" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="155" spans="1:11" ht="18">
       <c r="A155" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C155" s="3"/>
-      <c r="D155" s="3"/>
-      <c r="E155">
-        <v>359</v>
-      </c>
-      <c r="F155" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G155">
-        <v>1352</v>
-      </c>
-      <c r="H155" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="B155" s="5"/>
+      <c r="C155" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D155" s="5"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="H155" s="3"/>
       <c r="I155" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J155" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K155" s="3"/>
+      <c r="J155" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="156" spans="1:11" ht="18">
       <c r="A156" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>9</v>
+        <v>145</v>
+      </c>
+      <c r="B156" s="3">
+        <v>0</v>
       </c>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156">
-        <v>467</v>
+        <v>265</v>
       </c>
       <c r="F156" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G156">
-        <v>2956</v>
-      </c>
       <c r="H156" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J156" s="3" t="s">
-        <v>60</v>
+        <v>90</v>
+      </c>
+      <c r="J156" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="K156" s="3"/>
     </row>
     <row r="157" spans="1:11" ht="18">
       <c r="A157" s="3" t="s">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
-      <c r="E157" s="3"/>
-      <c r="F157" s="3"/>
-      <c r="G157" s="3"/>
-      <c r="H157" s="3"/>
+      <c r="E157">
+        <v>359</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G157">
+        <v>1352</v>
+      </c>
+      <c r="H157" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="I157" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="J157" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K157" s="3"/>
     </row>
     <row r="158" spans="1:11" ht="18">
       <c r="A158" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B158" s="4">
-        <v>58254</v>
-      </c>
-      <c r="C158" s="4"/>
-      <c r="D158" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3"/>
       <c r="E158">
-        <v>3850</v>
+        <v>467</v>
       </c>
       <c r="F158" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G158">
-        <v>502</v>
+        <v>2956</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="I158" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J158" s="3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="K158" s="3"/>
     </row>
     <row r="159" spans="1:11" ht="18">
-      <c r="A159" t="s">
-        <v>192</v>
-      </c>
+      <c r="A159" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159" s="3"/>
+      <c r="D159" s="3"/>
+      <c r="E159" s="3"/>
+      <c r="F159" s="3"/>
+      <c r="G159" s="3"/>
+      <c r="H159" s="3"/>
       <c r="I159" s="3" t="s">
         <v>34</v>
       </c>
       <c r="J159" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="K159" s="3"/>
     </row>
     <row r="160" spans="1:11" ht="18">
       <c r="A160" s="3" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B160" s="4">
-        <v>4022</v>
+        <v>58254</v>
       </c>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
       <c r="E160">
-        <v>2658</v>
+        <v>3850</v>
       </c>
       <c r="F160" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G160" s="3"/>
+      <c r="G160">
+        <v>502</v>
+      </c>
       <c r="H160" s="3" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="I160" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J160" s="3" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="K160" s="3"/>
     </row>
     <row r="161" spans="1:11" ht="18">
       <c r="A161" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="I161" s="3" t="s">
         <v>34</v>
@@ -5090,20 +5097,18 @@
     </row>
     <row r="162" spans="1:11" ht="18">
       <c r="A162" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C162" s="5"/>
-      <c r="D162" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E162" s="3">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="B162" s="4">
+        <v>4022</v>
+      </c>
+      <c r="C162" s="4"/>
+      <c r="D162" s="4"/>
+      <c r="E162">
+        <v>2658</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G162" s="3"/>
       <c r="H162" s="3" t="s">
@@ -5113,13 +5118,64 @@
         <v>10</v>
       </c>
       <c r="J162" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K162" s="3"/>
+    </row>
+    <row r="163" spans="1:11" ht="18">
+      <c r="A163" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I163" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J163" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" ht="18">
+      <c r="A164" t="s">
+        <v>176</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J164" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" ht="18">
+      <c r="A165" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C165" s="5"/>
+      <c r="D165" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E165" s="3">
+        <v>0</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G165" s="3"/>
+      <c r="H165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J165" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K162" s="3"/>
+      <c r="K165" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A3:K169">
-    <sortCondition ref="A3:A169"/>
+  <sortState ref="A2:K208">
+    <sortCondition ref="A2:A208"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>